<commit_message>
Worked on the frame. Optimized frame. Bom updated
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>S50MST-A07P50P50</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?vendor=0&amp;keywords=NAU7802KGI-ND</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/CanaKit-Raspberry-Basic-Clear-Supply/dp/B00DG9D6IK/ref=sr_1_6?ie=UTF8&amp;qid=1390244948&amp;sr=8-6&amp;keywords=raspberry+pi</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Samsung-S20B350H-20-Inch-LED-Lit-Monitor/dp/B007VPHS2U/ref=sr_1_7?ie=UTF8&amp;qid=1390245063&amp;sr=8-7&amp;keywords=hdmi+monitor</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/AmazonBasics-High-Speed-HDMI-Cable-Meters/dp/B003L1ZYYM/ref=sr_1_1?ie=UTF8&amp;qid=1390245092&amp;sr=8-1&amp;keywords=hdmi+cord</t>
+  </si>
+  <si>
+    <t>Darlington Array</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/312</t>
+  </si>
+  <si>
+    <t>Pressure Release</t>
+  </si>
+  <si>
+    <t>http://www.grainger.com/product/PRINCE-Relief-Valve-6X843?s_pp=false</t>
   </si>
 </sst>
 </file>
@@ -473,7 +497,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -502,6 +526,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,7 +542,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -602,10 +632,10 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>394.99</c:v>
+                  <c:v>397.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1182.75</c:v>
+                  <c:v>1261.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>340</c:v>
@@ -658,7 +688,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -968,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K41"/>
+  <dimension ref="B1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,16 +1039,16 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="24">
-        <f>SUM(F4:F12)</f>
-        <v>394.99</v>
+        <f>SUM(F4:F13)</f>
+        <v>397.99</v>
       </c>
       <c r="J3" s="8" t="str">
         <f>B3</f>
@@ -1026,7 +1056,7 @@
       </c>
       <c r="K3" s="20">
         <f>G3</f>
-        <v>394.99</v>
+        <v>397.99</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -1047,19 +1077,21 @@
         <v>24.990000000000002</v>
       </c>
       <c r="J4" s="8" t="str">
-        <f>B13</f>
+        <f>B14</f>
         <v>Hydrolics</v>
       </c>
       <c r="K4" s="20">
-        <f>G13</f>
-        <v>1182.75</v>
+        <f>G14</f>
+        <v>1261.25</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="34" t="s">
+        <v>36</v>
+      </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -1067,15 +1099,15 @@
         <v>50</v>
       </c>
       <c r="F5" s="9">
-        <f t="shared" ref="F5:F11" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F12" si="0">D5*E5</f>
         <v>50</v>
       </c>
       <c r="J5" s="8" t="str">
-        <f>B23</f>
+        <f>B25</f>
         <v>Mechanical</v>
       </c>
       <c r="K5" s="20">
-        <f>G23</f>
+        <f>G25</f>
         <v>340</v>
       </c>
     </row>
@@ -1083,7 +1115,9 @@
       <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="34" t="s">
+        <v>37</v>
+      </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
@@ -1095,11 +1129,11 @@
         <v>100</v>
       </c>
       <c r="J6" s="21" t="str">
-        <f>B33</f>
+        <f>B35</f>
         <v>Raw Materials</v>
       </c>
       <c r="K6" s="22">
-        <f>G33</f>
+        <f>G35</f>
         <v>498</v>
       </c>
     </row>
@@ -1107,7 +1141,9 @@
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
@@ -1123,23 +1159,25 @@
       </c>
       <c r="K7" s="27">
         <f>SUM(K3:K6)</f>
-        <v>2415.7399999999998</v>
+        <v>2497.2399999999998</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="D8" s="2">
         <v>5</v>
       </c>
       <c r="E8" s="3">
-        <v>4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -1174,153 +1212,161 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="9">
+    <row r="11" spans="2:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="30">
+        <v>6</v>
+      </c>
+      <c r="E11" s="31">
+        <v>2</v>
+      </c>
+      <c r="F11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13">
-        <f>D12*E12</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13">
+        <f>D13*E13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="24">
-        <f>SUM(F14:F22)</f>
-        <v>1182.75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="24">
+        <f>SUM(F15:F24)</f>
+        <v>1261.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E15" s="6">
         <v>171.75</v>
       </c>
-      <c r="F14" s="7">
-        <f>D14*E14</f>
+      <c r="F15" s="7">
+        <f>D15*E15</f>
         <v>171.75</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3">
-        <v>123</v>
-      </c>
-      <c r="F15" s="9">
-        <f t="shared" ref="F15:F21" si="1">D15*E15</f>
-        <v>123</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="3">
+        <v>123</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16:F23" si="1">D16*E16</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
         <v>236.5</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F17" s="9">
         <f t="shared" si="1"/>
         <v>236.5</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C18" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E18" s="26">
         <v>391.5</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F18" s="9">
         <f t="shared" si="1"/>
         <v>391.5</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
         <v>2</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E19" s="3">
         <v>100</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F19" s="9">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="9">
+    <row r="20" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="30">
+        <v>1</v>
+      </c>
+      <c r="E20" s="31">
+        <v>78.5</v>
+      </c>
+      <c r="F20" s="33">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>60</v>
-      </c>
-      <c r="F20" s="9">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1328,84 +1374,92 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="9">
+      <c r="F21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13">
-        <f>D22*E22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>60</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13">
+        <f>D24*E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="24">
-        <f>SUM(F24:F32)</f>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="24">
+        <f>SUM(F26:F34)</f>
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="5">
+      <c r="C26" s="18"/>
+      <c r="D26" s="5">
         <v>4</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E26" s="6">
         <v>10</v>
       </c>
-      <c r="F24" s="7">
-        <f>D24*E24</f>
+      <c r="F26" s="7">
+        <f>D26*E26</f>
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E27" s="3">
         <v>300</v>
       </c>
-      <c r="F25" s="9">
-        <f t="shared" ref="F25:F31" si="2">D25*E25</f>
+      <c r="F27" s="9">
+        <f t="shared" ref="F27:F33" si="2">D27*E27</f>
         <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1448,97 +1502,97 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13">
-        <f>D32*E32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="28" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13">
+        <f>D34*E34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="24">
-        <f>SUM(F34:F41)</f>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="24">
+        <f>SUM(F36:F43)</f>
         <v>498</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C36" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D36" s="5">
         <v>10</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E36" s="6">
         <v>42</v>
       </c>
-      <c r="F34" s="7">
-        <f>D34*E34</f>
+      <c r="F36" s="7">
+        <f>D36*E36</f>
         <v>420</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2">
         <v>4</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E37" s="3">
         <v>7</v>
       </c>
-      <c r="F35" s="9">
-        <f t="shared" ref="F35:F40" si="3">D35*E35</f>
+      <c r="F37" s="9">
+        <f t="shared" ref="F37:F42" si="3">D37*E37</f>
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E38" s="3">
         <v>50</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F38" s="9">
         <f t="shared" si="3"/>
         <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1561,33 +1615,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13">
-        <f>D41*E41</f>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="8"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="8"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13">
+        <f>D43*E43</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C16" r:id="rId2"/>
-    <hyperlink ref="C17" r:id="rId3"/>
-    <hyperlink ref="C34" r:id="rId4" location="6527k244/=pqk7y4" display="http://www.mcmaster.com/ - 6527k244/=pqk7y4"/>
-    <hyperlink ref="C15" r:id="rId5"/>
-    <hyperlink ref="C20" r:id="rId6" display="S50MST-A07P50P50 ()"/>
+    <hyperlink ref="C17" r:id="rId2"/>
+    <hyperlink ref="C18" r:id="rId3"/>
+    <hyperlink ref="C36" r:id="rId4" location="6527k244/=pqk7y4" display="http://www.mcmaster.com/ - 6527k244/=pqk7y4"/>
+    <hyperlink ref="C16" r:id="rId5"/>
+    <hyperlink ref="C22" r:id="rId6" display="S50MST-A07P50P50 ()"/>
+    <hyperlink ref="C15" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
+    <hyperlink ref="C6" r:id="rId10"/>
+    <hyperlink ref="C7" r:id="rId11"/>
+    <hyperlink ref="C11" r:id="rId12"/>
+    <hyperlink ref="C20" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
-  <drawing r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Hydraulic Design Updated BOM.xlsx with new parts
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="7935"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="10515" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,24 @@
   </si>
   <si>
     <t>http://www.grainger.com/product/PRINCE-Relief-Valve-6X843?s_pp=false</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>http://www.northerntool.com/shop/tools/product_200466862_200466862</t>
+  </si>
+  <si>
+    <t>http://www.northerntool.com/shop/tools/product_200339057_200339057?cm_mmc=Google-pla-_-Hydraulics-_-Hydraulic%20Valves-_-201615&amp;ci_src=17588969&amp;ci_sku=201615&amp;gclid=COWNt4KIk7wCFahj7AodkDEA_g</t>
+  </si>
+  <si>
+    <t>Better Valve</t>
+  </si>
+  <si>
+    <t>http://www.northerntool.com/shop/tools/product_472_472</t>
   </si>
 </sst>
 </file>
@@ -635,7 +653,7 @@
                   <c:v>397.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1261.25</c:v>
+                  <c:v>1337.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>340</c:v>
@@ -998,17 +1016,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K43"/>
+  <dimension ref="B1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" customWidth="1"/>
@@ -1082,7 +1101,7 @@
       </c>
       <c r="K4" s="20">
         <f>G14</f>
-        <v>1261.25</v>
+        <v>1337.75</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -1103,11 +1122,11 @@
         <v>50</v>
       </c>
       <c r="J5" s="8" t="str">
-        <f>B25</f>
+        <f>B28</f>
         <v>Mechanical</v>
       </c>
       <c r="K5" s="20">
-        <f>G25</f>
+        <f>G28</f>
         <v>340</v>
       </c>
     </row>
@@ -1129,11 +1148,11 @@
         <v>100</v>
       </c>
       <c r="J6" s="21" t="str">
-        <f>B35</f>
+        <f>B38</f>
         <v>Raw Materials</v>
       </c>
       <c r="K6" s="22">
-        <f>G35</f>
+        <f>G38</f>
         <v>498</v>
       </c>
     </row>
@@ -1159,7 +1178,7 @@
       </c>
       <c r="K7" s="27">
         <f>SUM(K3:K6)</f>
-        <v>2497.2399999999998</v>
+        <v>2573.7399999999998</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1259,8 +1278,8 @@
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
       <c r="G14" s="24">
-        <f>SUM(F15:F24)</f>
-        <v>1261.25</v>
+        <f>SUM(F15:F27)</f>
+        <v>1337.75</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -1295,7 +1314,7 @@
         <v>123</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" ref="F16:F23" si="1">D16*E16</f>
+        <f t="shared" ref="F16:F26" si="1">D16*E16</f>
         <v>123</v>
       </c>
     </row>
@@ -1359,137 +1378,161 @@
         <v>42</v>
       </c>
       <c r="D20" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="31">
         <v>78.5</v>
       </c>
       <c r="F20" s="33">
         <f t="shared" si="1"/>
-        <v>78.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="30">
+        <v>0</v>
+      </c>
+      <c r="E21" s="31">
+        <v>115</v>
+      </c>
       <c r="F21" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="30">
+        <v>1</v>
+      </c>
+      <c r="E22" s="31">
+        <v>85</v>
+      </c>
+      <c r="F22" s="33">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1</v>
+      </c>
+      <c r="E23" s="31">
+        <v>70</v>
+      </c>
+      <c r="F23" s="33">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D25" s="2">
         <v>1</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E25" s="3">
         <v>60</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F25" s="33">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="9">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13">
-        <f>D24*E24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="35" t="s">
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13">
+        <f>D27*E27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="24">
-        <f>SUM(F26:F34)</f>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="24">
+        <f>SUM(F29:F37)</f>
         <v>340</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="5">
+      <c r="C29" s="18"/>
+      <c r="D29" s="5">
         <v>4</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E29" s="6">
         <v>10</v>
       </c>
-      <c r="F26" s="7">
-        <f>D26*E26</f>
+      <c r="F29" s="7">
+        <f>D29*E29</f>
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
         <v>1</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E30" s="3">
         <v>300</v>
       </c>
-      <c r="F27" s="9">
-        <f t="shared" ref="F27:F33" si="2">D27*E27</f>
+      <c r="F30" s="9">
+        <f t="shared" ref="F30:F36" si="2">D30*E30</f>
         <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1522,107 +1565,107 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13">
-        <f>D34*E34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="35" t="s">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13">
+        <f>D37*E37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="24">
-        <f>SUM(F36:F43)</f>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="24">
+        <f>SUM(F39:F46)</f>
         <v>498</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C39" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D39" s="5">
         <v>10</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E39" s="6">
         <v>42</v>
       </c>
-      <c r="F36" s="7">
-        <f>D36*E36</f>
+      <c r="F39" s="7">
+        <f>D39*E39</f>
         <v>420</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2">
         <v>4</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E40" s="3">
         <v>7</v>
       </c>
-      <c r="F37" s="9">
-        <f t="shared" ref="F37:F42" si="3">D37*E37</f>
+      <c r="F40" s="9">
+        <f t="shared" ref="F40:F45" si="3">D40*E40</f>
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2">
         <v>1</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E41" s="3">
         <v>50</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F41" s="9">
         <f t="shared" si="3"/>
         <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
@@ -1635,13 +1678,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13">
-        <f>D43*E43</f>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="8"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="8"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="8"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13">
+        <f>D46*E46</f>
         <v>0</v>
       </c>
     </row>
@@ -1649,16 +1722,16 @@
   <mergeCells count="4">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B38:F38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C17" r:id="rId2"/>
     <hyperlink ref="C18" r:id="rId3"/>
-    <hyperlink ref="C36" r:id="rId4" location="6527k244/=pqk7y4" display="http://www.mcmaster.com/ - 6527k244/=pqk7y4"/>
+    <hyperlink ref="C39" r:id="rId4" location="6527k244/=pqk7y4" display="http://www.mcmaster.com/ - 6527k244/=pqk7y4"/>
     <hyperlink ref="C16" r:id="rId5"/>
-    <hyperlink ref="C22" r:id="rId6" display="S50MST-A07P50P50 ()"/>
+    <hyperlink ref="C25" r:id="rId6" display="S50MST-A07P50P50 ()"/>
     <hyperlink ref="C15" r:id="rId7"/>
     <hyperlink ref="C8" r:id="rId8"/>
     <hyperlink ref="C5" r:id="rId9"/>

</xml_diff>

<commit_message>
Updated the BOM.xlsx Started on a Force Sensor Diagram
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -64,9 +64,6 @@
     <t>http://www.grainger.com/product/MAXIM-Hydraulic-Cylinder-6FDA8?Pid=search</t>
   </si>
   <si>
-    <t>Sensor</t>
-  </si>
-  <si>
     <t>http://www.instrumart.com/products/30859/ashcroft-a2-heavy-industrial-pressure-transmitter?gclid=CNm0wdGv9LoCFU4OOgod_VEAbg</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>http://www.northerntool.com/shop/tools/product_472_472</t>
+  </si>
+  <si>
+    <t>Sensor (0-5V)</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -679,7 +678,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1018,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,10 +1104,10 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1132,10 +1130,10 @@
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1158,10 +1156,10 @@
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1183,10 +1181,10 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -1201,7 +1199,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
@@ -1217,7 +1215,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
@@ -1233,10 +1231,10 @@
     </row>
     <row r="11" spans="2:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>40</v>
       </c>
       <c r="D11" s="30">
         <v>6</v>
@@ -1287,7 +1285,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -1305,7 +1303,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1338,10 +1336,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="25" t="s">
         <v>16</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>17</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1356,7 +1354,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
@@ -1372,10 +1370,10 @@
     </row>
     <row r="20" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>41</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>42</v>
       </c>
       <c r="D20" s="30">
         <v>0</v>
@@ -1390,10 +1388,10 @@
     </row>
     <row r="21" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="30">
         <v>0</v>
@@ -1408,10 +1406,10 @@
     </row>
     <row r="22" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="34" t="s">
         <v>47</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>48</v>
       </c>
       <c r="D22" s="30">
         <v>1</v>
@@ -1426,10 +1424,10 @@
     </row>
     <row r="23" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="34" t="s">
         <v>44</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>45</v>
       </c>
       <c r="D23" s="30">
         <v>1</v>
@@ -1454,10 +1452,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>34</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -1505,7 +1503,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="5">
@@ -1521,7 +1519,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2">
@@ -1620,10 +1618,10 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>21</v>
       </c>
       <c r="D39" s="5">
         <v>10</v>
@@ -1638,7 +1636,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2">
@@ -1654,7 +1652,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -1739,9 +1737,10 @@
     <hyperlink ref="C7" r:id="rId11"/>
     <hyperlink ref="C11" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
+    <hyperlink ref="C23" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
-  <drawing r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a filter to the Hydraulic.pptx Design added a steel BOM.txt converted the frame reports to PDF. Deleted the extra Solidworks folder. (Some files are still read only and I can't delete them.)
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -40,9 +40,6 @@
     <t>Electronics</t>
   </si>
   <si>
-    <t>Hydrolics</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>S50MST-A07P50P50</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?vendor=0&amp;keywords=NAU7802KGI-ND</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/CanaKit-Raspberry-Basic-Clear-Supply/dp/B00DG9D6IK/ref=sr_1_6?ie=UTF8&amp;qid=1390244948&amp;sr=8-6&amp;keywords=raspberry+pi</t>
   </si>
   <si>
@@ -161,6 +155,12 @@
   </si>
   <si>
     <t>Sensor (0-5V)</t>
+  </si>
+  <si>
+    <t>http://www.adafruit.com/products/1085</t>
+  </si>
+  <si>
+    <t>Hydraulics</t>
   </si>
 </sst>
 </file>
@@ -591,6 +591,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -631,7 +632,7 @@
                   <c:v>Electronics</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Hydrolics</c:v>
+                  <c:v>Hydraulics</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Mechanical</c:v>
@@ -649,10 +650,10 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>397.99</c:v>
+                  <c:v>431.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1337.75</c:v>
+                  <c:v>1137.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>340</c:v>
@@ -678,6 +679,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1017,7 +1019,7 @@
   <dimension ref="B1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B14" sqref="B14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>5</v>
@@ -1065,7 +1067,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="24">
         <f>SUM(F4:F13)</f>
-        <v>397.99</v>
+        <v>431.84000000000003</v>
       </c>
       <c r="J3" s="8" t="str">
         <f>B3</f>
@@ -1073,7 +1075,7 @@
       </c>
       <c r="K3" s="20">
         <f>G3</f>
-        <v>397.99</v>
+        <v>431.84000000000003</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -1095,19 +1097,19 @@
       </c>
       <c r="J4" s="8" t="str">
         <f>B14</f>
-        <v>Hydrolics</v>
+        <v>Hydraulics</v>
       </c>
       <c r="K4" s="20">
         <f>G14</f>
-        <v>1337.75</v>
+        <v>1137.75</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1130,10 +1132,10 @@
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1156,10 +1158,10 @@
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1176,30 +1178,30 @@
       </c>
       <c r="K7" s="27">
         <f>SUM(K3:K6)</f>
-        <v>2573.7399999999998</v>
+        <v>2407.59</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="D8" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>2.2000000000000002</v>
+        <v>14.95</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>44.849999999999994</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
@@ -1215,7 +1217,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
@@ -1231,10 +1233,10 @@
     </row>
     <row r="11" spans="2:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="30">
         <v>6</v>
@@ -1269,7 +1271,7 @@
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="35" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
@@ -1277,15 +1279,15 @@
       <c r="F14" s="37"/>
       <c r="G14" s="24">
         <f>SUM(F15:F27)</f>
-        <v>1337.75</v>
+        <v>1137.75</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -1300,10 +1302,10 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1318,10 +1320,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="25" t="s">
         <v>14</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>15</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1336,10 +1338,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1354,26 +1356,24 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2">
-        <v>2</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="3">
         <v>100</v>
       </c>
       <c r="F19" s="9">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="30">
         <v>0</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="21" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="30">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="22" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="30">
         <v>1</v>
@@ -1424,10 +1424,10 @@
     </row>
     <row r="23" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" s="30">
         <v>1</v>
@@ -1452,10 +1452,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>32</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>33</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="5">
@@ -1519,7 +1519,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2">
@@ -1605,7 +1605,7 @@
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C38" s="36"/>
       <c r="D38" s="36"/>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>20</v>
       </c>
       <c r="D39" s="5">
         <v>10</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2">
@@ -1652,7 +1652,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -1731,13 +1731,13 @@
     <hyperlink ref="C16" r:id="rId5"/>
     <hyperlink ref="C25" r:id="rId6" display="S50MST-A07P50P50 ()"/>
     <hyperlink ref="C15" r:id="rId7"/>
-    <hyperlink ref="C8" r:id="rId8"/>
-    <hyperlink ref="C5" r:id="rId9"/>
-    <hyperlink ref="C6" r:id="rId10"/>
-    <hyperlink ref="C7" r:id="rId11"/>
-    <hyperlink ref="C11" r:id="rId12"/>
-    <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C23" r:id="rId14"/>
+    <hyperlink ref="C5" r:id="rId8"/>
+    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="C7" r:id="rId10"/>
+    <hyperlink ref="C11" r:id="rId11"/>
+    <hyperlink ref="C20" r:id="rId12"/>
+    <hyperlink ref="C23" r:id="rId13"/>
+    <hyperlink ref="C8" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>

<commit_message>
Added steel lists to the bom.
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -73,9 +74,6 @@
     <t>Frame Steel</t>
   </si>
   <si>
-    <t>http://www.mcmaster.com/#6527k244/=pqk7y4</t>
-  </si>
-  <si>
     <t>Castors</t>
   </si>
   <si>
@@ -161,15 +159,50 @@
   </si>
   <si>
     <t>Hydraulics</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>http://www.grainger.com/product/Spin-on-Filter-3KML8?s_pp=false</t>
+  </si>
+  <si>
+    <t>Filter Replacement</t>
+  </si>
+  <si>
+    <t>http://www.grainger.com/product/PARKER-Filter-Element-1R412?opr=OAPD&amp;pbi=3KML8</t>
+  </si>
+  <si>
+    <t>http://www.capitalsteel.net/</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Dimensional</t>
+  </si>
+  <si>
+    <t>2x2x 1/8</t>
+  </si>
+  <si>
+    <t>3x3x 1/8</t>
+  </si>
+  <si>
+    <t>3x6x 1/8</t>
+  </si>
+  <si>
+    <t>Steel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#.0\ &quot;in&quot;"/>
+    <numFmt numFmtId="165" formatCode="#.00\ &quot;ft&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -219,7 +252,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -498,6 +531,60 @@
     </border>
     <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -515,7 +602,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -560,6 +647,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -653,13 +767,13 @@
                   <c:v>431.84000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1137.75</c:v>
+                  <c:v>1217.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>498</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1016,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K46"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1215,7 @@
       </c>
       <c r="K4" s="20">
         <f>G14</f>
-        <v>1137.75</v>
+        <v>1217.75</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -1109,7 +1223,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1122,11 +1236,11 @@
         <v>50</v>
       </c>
       <c r="J5" s="8" t="str">
-        <f>B28</f>
+        <f>B30</f>
         <v>Mechanical</v>
       </c>
       <c r="K5" s="20">
-        <f>G28</f>
+        <f>G30</f>
         <v>340</v>
       </c>
     </row>
@@ -1135,7 +1249,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1148,20 +1262,20 @@
         <v>100</v>
       </c>
       <c r="J6" s="21" t="str">
-        <f>B38</f>
+        <f>B40</f>
         <v>Raw Materials</v>
       </c>
       <c r="K6" s="22">
-        <f>G38</f>
-        <v>498</v>
+        <f>G40</f>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1178,15 +1292,15 @@
       </c>
       <c r="K7" s="27">
         <f>SUM(K3:K6)</f>
-        <v>2407.59</v>
+        <v>2067.59</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -1201,7 +1315,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
@@ -1217,7 +1331,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
@@ -1233,10 +1347,10 @@
     </row>
     <row r="11" spans="2:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>37</v>
       </c>
       <c r="D11" s="30">
         <v>6</v>
@@ -1271,15 +1385,15 @@
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
       <c r="G14" s="24">
-        <f>SUM(F15:F27)</f>
-        <v>1137.75</v>
+        <f>SUM(F15:F29)</f>
+        <v>1217.75</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -1287,7 +1401,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -1305,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1314,11 +1428,11 @@
         <v>123</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" ref="F16:F26" si="1">D16*E16</f>
+        <f t="shared" ref="F16:F28" si="1">D16*E16</f>
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>13</v>
       </c>
@@ -1336,9 +1450,9 @@
         <v>236.5</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>15</v>
@@ -1354,9 +1468,9 @@
         <v>391.5</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1368,12 +1482,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>39</v>
       </c>
       <c r="D20" s="30">
         <v>0</v>
@@ -1386,12 +1500,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="30">
         <v>0</v>
@@ -1404,12 +1518,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="34" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>45</v>
       </c>
       <c r="D22" s="30">
         <v>1</v>
@@ -1422,12 +1536,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="2:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="34" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="30">
         <v>1</v>
@@ -1440,120 +1554,155 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
+    <row r="24" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="30">
+        <v>1</v>
+      </c>
+      <c r="E24" s="31">
+        <v>40</v>
+      </c>
       <c r="F24" s="33">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>60</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="30">
+        <v>2</v>
+      </c>
+      <c r="E25" s="31">
+        <v>20</v>
       </c>
       <c r="F25" s="33">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="9">
+      <c r="F26" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13">
-        <f>D27*E27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>60</v>
+      </c>
+      <c r="F27" s="33">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13">
+        <f>D29*E29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="24">
-        <f>SUM(F29:F37)</f>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="24">
+        <f>SUM(F31:F39)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="5">
+      <c r="K30" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="L30" s="42"/>
+      <c r="M30" s="43"/>
+    </row>
+    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="5">
         <v>4</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E31" s="6">
         <v>10</v>
       </c>
-      <c r="F29" s="7">
-        <f>D29*E29</f>
+      <c r="F31" s="7">
+        <f>D31*E31</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2">
+      <c r="K31" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="L31" s="42"/>
+      <c r="M31" s="43"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2">
         <v>1</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E32" s="3">
         <v>300</v>
       </c>
-      <c r="F30" s="9">
-        <f t="shared" ref="F30:F36" si="2">D30*E30</f>
+      <c r="F32" s="9">
+        <f t="shared" ref="F32:F38" si="2">D32*E32</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K32" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="L32" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1562,8 +1711,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K33" s="44">
+        <v>30</v>
+      </c>
+      <c r="L33" s="44">
+        <v>32</v>
+      </c>
+      <c r="M33" s="44">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1572,8 +1730,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K34" s="44">
+        <v>30</v>
+      </c>
+      <c r="L34" s="44">
+        <v>32</v>
+      </c>
+      <c r="M34" s="44"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1582,8 +1747,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K35" s="44">
+        <v>30</v>
+      </c>
+      <c r="L35" s="44">
+        <v>65</v>
+      </c>
+      <c r="M35" s="44"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1592,155 +1764,358 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13">
-        <f>D37*E37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="35" t="s">
+      <c r="K36" s="44">
+        <v>30</v>
+      </c>
+      <c r="L36" s="44">
+        <v>65</v>
+      </c>
+      <c r="M36" s="44"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="44">
+        <v>30</v>
+      </c>
+      <c r="L37" s="44">
+        <v>73.5</v>
+      </c>
+      <c r="M37" s="44"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="44">
+        <v>30</v>
+      </c>
+      <c r="L38" s="44">
+        <v>73.5</v>
+      </c>
+      <c r="M38" s="44"/>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13">
+        <f>D39*E39</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="44">
+        <v>8</v>
+      </c>
+      <c r="L39" s="44">
+        <v>120</v>
+      </c>
+      <c r="M39" s="44"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="24">
-        <f>SUM(F39:F46)</f>
-        <v>498</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="24">
+        <f>SUM(F41:F54)</f>
+        <v>78</v>
+      </c>
+      <c r="K40" s="44">
+        <v>8</v>
+      </c>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="5">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6">
-        <v>42</v>
-      </c>
-      <c r="F39" s="7">
-        <f>D39*E39</f>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+      <c r="C41" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <f>D41*E41</f>
+        <v>0</v>
+      </c>
+      <c r="K41" s="44">
+        <v>8</v>
+      </c>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="40" t="str">
+        <f>K32</f>
+        <v>2x2x 1/8</v>
+      </c>
+      <c r="C42" s="30"/>
+      <c r="D42" s="48">
+        <f>K47</f>
+        <v>23</v>
+      </c>
+      <c r="E42" s="31">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33">
+        <f t="shared" ref="F42:F47" si="3">D42*E42</f>
+        <v>0</v>
+      </c>
+      <c r="K42" s="44">
+        <v>8</v>
+      </c>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="40" t="str">
+        <f>L32</f>
+        <v>3x3x 1/8</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="48">
+        <f>L47</f>
+        <v>38.416666666666664</v>
+      </c>
+      <c r="E43" s="31">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="44">
+        <v>16</v>
+      </c>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+    </row>
+    <row r="44" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="40" t="str">
+        <f>M32</f>
+        <v>3x6x 1/8</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="D44" s="48">
+        <f>M47</f>
+        <v>4.75</v>
+      </c>
+      <c r="E44" s="31">
+        <v>0</v>
+      </c>
+      <c r="F44" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="44">
+        <v>16</v>
+      </c>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+    </row>
+    <row r="45" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="31">
+        <v>0</v>
+      </c>
+      <c r="F45" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="44">
+        <v>16</v>
+      </c>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+    </row>
+    <row r="46" spans="1:13" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="38"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="31">
+        <v>0</v>
+      </c>
+      <c r="F46" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="45">
+        <v>16</v>
+      </c>
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
+    </row>
+    <row r="47" spans="1:13" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="40"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="31">
+        <v>0</v>
+      </c>
+      <c r="F47" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="46">
+        <f>SUM(K33:K46)/12</f>
+        <v>23</v>
+      </c>
+      <c r="L47" s="46">
+        <f>SUM(L33:L46)/12</f>
+        <v>38.416666666666664</v>
+      </c>
+      <c r="M47" s="46">
+        <f>SUM(M33:M46)/12</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2">
+        <v>4</v>
+      </c>
+      <c r="E48" s="3">
+        <v>7</v>
+      </c>
+      <c r="F48" s="9">
+        <f t="shared" ref="F48:F53" si="4">D48*E48</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2">
-        <v>4</v>
-      </c>
-      <c r="E40" s="3">
-        <v>7</v>
-      </c>
-      <c r="F40" s="9">
-        <f t="shared" ref="F40:F45" si="3">D40*E40</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2">
         <v>1</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E49" s="3">
         <v>50</v>
       </c>
-      <c r="F41" s="9">
-        <f t="shared" si="3"/>
+      <c r="F49" s="9">
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="8"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="10"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13">
-        <f>D46*E46</f>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="8"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="8"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="8"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="13">
+        <f>D54*E54</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="K30:M30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C17" r:id="rId2"/>
     <hyperlink ref="C18" r:id="rId3"/>
-    <hyperlink ref="C39" r:id="rId4" location="6527k244/=pqk7y4" display="http://www.mcmaster.com/ - 6527k244/=pqk7y4"/>
-    <hyperlink ref="C16" r:id="rId5"/>
-    <hyperlink ref="C25" r:id="rId6" display="S50MST-A07P50P50 ()"/>
-    <hyperlink ref="C15" r:id="rId7"/>
-    <hyperlink ref="C5" r:id="rId8"/>
-    <hyperlink ref="C6" r:id="rId9"/>
-    <hyperlink ref="C7" r:id="rId10"/>
-    <hyperlink ref="C11" r:id="rId11"/>
-    <hyperlink ref="C20" r:id="rId12"/>
-    <hyperlink ref="C23" r:id="rId13"/>
-    <hyperlink ref="C8" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId4"/>
+    <hyperlink ref="C27" r:id="rId5" display="S50MST-A07P50P50 ()"/>
+    <hyperlink ref="C15" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C20" r:id="rId11"/>
+    <hyperlink ref="C23" r:id="rId12"/>
+    <hyperlink ref="C8" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM to have shipping Updated hydraulics to include filter
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="165" windowWidth="10515" windowHeight="7875"/>
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -116,9 +116,6 @@
     <t>http://www.amazon.com/CanaKit-Raspberry-Basic-Clear-Supply/dp/B00DG9D6IK/ref=sr_1_6?ie=UTF8&amp;qid=1390244948&amp;sr=8-6&amp;keywords=raspberry+pi</t>
   </si>
   <si>
-    <t>http://www.amazon.com/Samsung-S20B350H-20-Inch-LED-Lit-Monitor/dp/B007VPHS2U/ref=sr_1_7?ie=UTF8&amp;qid=1390245063&amp;sr=8-7&amp;keywords=hdmi+monitor</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/AmazonBasics-High-Speed-HDMI-Cable-Meters/dp/B003L1ZYYM/ref=sr_1_1?ie=UTF8&amp;qid=1390245092&amp;sr=8-1&amp;keywords=hdmi+cord</t>
   </si>
   <si>
@@ -192,6 +189,18 @@
   </si>
   <si>
     <t>Steel</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Asus-VE228H-21-5-Inch-Integrated-Speakers/dp/B00413PHDM/ref=sr_1_8?ie=UTF8&amp;qid=1390944630&amp;sr=8-8&amp;keywords=hdmi+computer+monitor</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/Protronix-External-Portable-Drive-Black/dp/B004CG1UCK/ref=sr_1_4?s=electronics&amp;ie=UTF8&amp;qid=1390943913&amp;sr=1-4&amp;keywords=external+hard+drive</t>
+  </si>
+  <si>
+    <t>USB external HDD</t>
+  </si>
+  <si>
+    <t>Shipping</t>
   </si>
 </sst>
 </file>
@@ -252,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -590,6 +599,144 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -602,17 +749,14 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
@@ -625,41 +769,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -674,6 +797,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -718,7 +884,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$2</c:f>
+              <c:f>Sheet1!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -739,9 +905,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$3:$J$6</c:f>
+              <c:f>Sheet1!$K$3:$K$5</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Electronics</c:v>
                 </c:pt>
@@ -751,29 +917,23 @@
                 <c:pt idx="2">
                   <c:v>Mechanical</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Raw Materials</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$6</c:f>
+              <c:f>Sheet1!$L$3:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>431.84000000000003</c:v>
+                  <c:v>485.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1217.75</c:v>
+                  <c:v>1742.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,13 +972,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1130,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,949 +1301,1033 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="24">
-        <f>SUM(F4:F13)</f>
-        <v>431.84000000000003</v>
-      </c>
-      <c r="J3" s="8" t="str">
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="20">
+        <f>SUM(G4:G13)</f>
+        <v>485.45</v>
+      </c>
+      <c r="K3" s="6" t="str">
         <f>B3</f>
         <v>Electronics</v>
       </c>
-      <c r="K3" s="20">
-        <f>G3</f>
-        <v>431.84000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="L3" s="17">
+        <f>H3</f>
+        <v>485.45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
-        <v>10</v>
-      </c>
-      <c r="E4" s="6">
-        <v>2.4990000000000001</v>
-      </c>
-      <c r="F4" s="7">
-        <f>D4*E4</f>
-        <v>24.990000000000002</v>
-      </c>
-      <c r="J4" s="8" t="str">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>25</v>
+      </c>
+      <c r="F4" s="46">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <f>(D4*E4)+F4</f>
+        <v>25</v>
+      </c>
+      <c r="K4" s="6" t="str">
         <f>B14</f>
         <v>Hydraulics</v>
       </c>
-      <c r="K4" s="20">
-        <f>G14</f>
-        <v>1217.75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="L4" s="17">
+        <f>H14</f>
+        <v>1742.07</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
-        <v>50</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5:F12" si="0">D5*E5</f>
-        <v>50</v>
-      </c>
-      <c r="J5" s="8" t="str">
+      <c r="E5" s="25">
+        <v>55</v>
+      </c>
+      <c r="F5" s="47">
+        <v>12.72</v>
+      </c>
+      <c r="G5" s="27">
+        <f t="shared" ref="G5:G12" si="0">(D5*E5)+F5</f>
+        <v>67.72</v>
+      </c>
+      <c r="K5" s="6" t="str">
         <f>B30</f>
         <v>Mechanical</v>
       </c>
-      <c r="K5" s="20">
-        <f>G30</f>
+      <c r="L5" s="17">
+        <f>H30</f>
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:12" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="24">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
+        <v>136</v>
+      </c>
+      <c r="F6" s="47">
+        <v>0</v>
+      </c>
+      <c r="G6" s="27">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="K6" s="37"/>
+      <c r="L6" s="38"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="24">
         <v>1</v>
       </c>
-      <c r="E6" s="3">
-        <v>100</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="E7" s="25">
+        <v>5.79</v>
+      </c>
+      <c r="F7" s="47">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="J6" s="21" t="str">
-        <f>B40</f>
-        <v>Raw Materials</v>
-      </c>
-      <c r="K6" s="22">
-        <f>G40</f>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="2">
+        <v>5.79</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="22">
+        <f>SUM(L3:L5)</f>
+        <v>2567.52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
-        <v>20</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E8" s="25">
+        <v>14.95</v>
+      </c>
+      <c r="F8" s="47">
+        <v>4.07</v>
+      </c>
+      <c r="G8" s="27">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J7" s="23" t="s">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24">
+        <v>6</v>
+      </c>
+      <c r="E9" s="25">
         <v>5</v>
       </c>
-      <c r="K7" s="27">
-        <f>SUM(K3:K6)</f>
-        <v>2067.59</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3">
-        <v>14.95</v>
-      </c>
-      <c r="F8" s="9">
-        <f t="shared" si="0"/>
-        <v>44.849999999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="F9" s="47"/>
+      <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24">
         <v>1</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="25">
         <v>150</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="47"/>
+      <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="2:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="32" t="s">
+    <row r="11" spans="2:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="30">
+      <c r="D11" s="24">
         <v>6</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="25">
         <v>2</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="47">
+        <v>4.43</v>
+      </c>
+      <c r="G11" s="27">
         <f t="shared" si="0"/>
+        <v>16.43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25">
+        <v>28</v>
+      </c>
+      <c r="F12" s="47">
+        <v>7.49</v>
+      </c>
+      <c r="G12" s="27">
+        <f t="shared" si="0"/>
+        <v>35.49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60">
+        <f>D13*E13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="52">
+        <f>SUM(G15:G29)</f>
+        <v>1742.07</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13">
-        <f>D13*E13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="24">
-        <f>SUM(F15:F29)</f>
-        <v>1217.75</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="30">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="50">
         <v>171.75</v>
       </c>
-      <c r="F15" s="7">
-        <f>D15*E15</f>
-        <v>171.75</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="F15" s="51">
+        <v>24.32</v>
+      </c>
+      <c r="G15" s="56">
+        <f>(D15*E15)+F15</f>
+        <v>196.07</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="24">
         <v>1</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="25">
         <v>123</v>
       </c>
-      <c r="F16" s="9">
-        <f t="shared" ref="F16:F28" si="1">D16*E16</f>
+      <c r="F16" s="47"/>
+      <c r="G16" s="27">
+        <f t="shared" ref="G16:G28" si="1">(D16*E16)+F16</f>
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="24">
         <v>1</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="25">
         <v>236.5</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="47">
+        <v>0</v>
+      </c>
+      <c r="G17" s="27">
         <f t="shared" si="1"/>
         <v>236.5</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="25" t="s">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="24">
         <v>1</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="21">
         <v>391.5</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="47"/>
+      <c r="G18" s="27">
         <f t="shared" si="1"/>
         <v>391.5</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24">
+        <v>5</v>
+      </c>
+      <c r="E19" s="25">
         <v>100</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="47"/>
+      <c r="G19" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="32" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="24">
+        <v>0</v>
+      </c>
+      <c r="E20" s="25">
+        <v>78.5</v>
+      </c>
+      <c r="F20" s="47">
+        <v>0</v>
+      </c>
+      <c r="G20" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="30">
-        <v>0</v>
-      </c>
-      <c r="E20" s="31">
-        <v>78.5</v>
-      </c>
-      <c r="F20" s="33">
+      <c r="C21" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="25">
+        <v>115</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="34" t="s">
+    <row r="22" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="30">
-        <v>0</v>
-      </c>
-      <c r="E21" s="31">
-        <v>115</v>
-      </c>
-      <c r="F21" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="C22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="30">
+      <c r="D22" s="24">
         <v>1</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="25">
         <v>85</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="47"/>
+      <c r="G22" s="27">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="32" t="s">
+    <row r="23" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="30">
+      <c r="D23" s="24">
         <v>1</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="25">
         <v>70</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="47"/>
+      <c r="G23" s="27">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+    <row r="24" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="30">
+      <c r="D24" s="24">
         <v>1</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="25">
         <v>40</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="47">
+        <v>0</v>
+      </c>
+      <c r="G24" s="27">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="32" t="s">
+    <row r="25" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="30">
+      <c r="D25" s="24">
         <v>2</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="25">
         <v>20</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="47">
+        <v>0</v>
+      </c>
+      <c r="G25" s="27">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="33">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="26"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="24">
         <v>1</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="25">
         <v>60</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="47"/>
+      <c r="G27" s="27">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="9">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="26"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13">
+    <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="18"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60">
         <f>D29*E29</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="35" t="s">
+    <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="24">
-        <f>SUM(F31:F39)</f>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="52">
+        <f>SUM(G31:G39)</f>
         <v>340</v>
       </c>
-      <c r="K30" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="L30" s="42"/>
+      <c r="L30" s="42" t="s">
+        <v>57</v>
+      </c>
       <c r="M30" s="43"/>
-    </row>
-    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="4" t="s">
+      <c r="N30" s="44"/>
+    </row>
+    <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="5">
+      <c r="C31" s="61"/>
+      <c r="D31" s="30">
         <v>4</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="50">
         <v>10</v>
       </c>
-      <c r="F31" s="7">
-        <f>D31*E31</f>
+      <c r="F31" s="51"/>
+      <c r="G31" s="56">
+        <f>(D31*E31)+F31</f>
         <v>40</v>
       </c>
-      <c r="K31" s="41" t="s">
+      <c r="L31" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="M31" s="43"/>
+      <c r="N31" s="44"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24">
+        <v>1</v>
+      </c>
+      <c r="E32" s="25">
+        <v>300</v>
+      </c>
+      <c r="F32" s="47"/>
+      <c r="G32" s="27">
+        <f t="shared" ref="G32:G39" si="2">(D32*E32)+F32</f>
+        <v>300</v>
+      </c>
+      <c r="L32" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="42"/>
-      <c r="M31" s="43"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2">
+      <c r="M32" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="26"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="32">
+        <v>30</v>
+      </c>
+      <c r="M33" s="32">
+        <v>32</v>
+      </c>
+      <c r="N33" s="32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="26"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="32">
+        <v>30</v>
+      </c>
+      <c r="M34" s="32">
+        <v>32</v>
+      </c>
+      <c r="N34" s="32"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="26"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="32">
+        <v>30</v>
+      </c>
+      <c r="M35" s="32">
+        <v>65</v>
+      </c>
+      <c r="N35" s="32"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="26"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="32">
+        <v>30</v>
+      </c>
+      <c r="M36" s="32">
+        <v>65</v>
+      </c>
+      <c r="N36" s="32"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="26"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="32">
+        <v>30</v>
+      </c>
+      <c r="M37" s="32">
+        <v>73.5</v>
+      </c>
+      <c r="N37" s="32"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="26"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L38" s="32">
+        <v>30</v>
+      </c>
+      <c r="M38" s="32">
+        <v>73.5</v>
+      </c>
+      <c r="N38" s="32"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="18"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="32">
+        <v>8</v>
+      </c>
+      <c r="M39" s="32">
+        <v>120</v>
+      </c>
+      <c r="N39" s="32"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="52">
+        <f>SUM(G41:G54)</f>
+        <v>78</v>
+      </c>
+      <c r="L40" s="32">
+        <v>8</v>
+      </c>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="30">
+        <v>0</v>
+      </c>
+      <c r="E41" s="50">
+        <v>0</v>
+      </c>
+      <c r="F41" s="50"/>
+      <c r="G41" s="56">
+        <f>(E41*D41)+F41</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="32">
+        <v>8</v>
+      </c>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+    </row>
+    <row r="42" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="31" t="str">
+        <f>L32</f>
+        <v>2x2x 1/8</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="36">
+        <f>L47</f>
+        <v>23</v>
+      </c>
+      <c r="E42" s="25">
+        <v>0</v>
+      </c>
+      <c r="F42" s="47"/>
+      <c r="G42" s="27">
+        <f t="shared" ref="G42:G54" si="3">(E42*D42)+F42</f>
+        <v>0</v>
+      </c>
+      <c r="L42" s="32">
+        <v>8</v>
+      </c>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+    </row>
+    <row r="43" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="31" t="str">
+        <f>M32</f>
+        <v>3x3x 1/8</v>
+      </c>
+      <c r="C43" s="24"/>
+      <c r="D43" s="36">
+        <f>M47</f>
+        <v>38.416666666666664</v>
+      </c>
+      <c r="E43" s="25">
+        <v>0</v>
+      </c>
+      <c r="F43" s="47"/>
+      <c r="G43" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="32">
+        <v>16</v>
+      </c>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+    </row>
+    <row r="44" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="31" t="str">
+        <f>N32</f>
+        <v>3x6x 1/8</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="36">
+        <f>N47</f>
+        <v>4.75</v>
+      </c>
+      <c r="E44" s="25">
+        <v>0</v>
+      </c>
+      <c r="F44" s="47"/>
+      <c r="G44" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="32">
+        <v>16</v>
+      </c>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+    </row>
+    <row r="45" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="29"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="25">
+        <v>0</v>
+      </c>
+      <c r="F45" s="47"/>
+      <c r="G45" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="32">
+        <v>16</v>
+      </c>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+    </row>
+    <row r="46" spans="1:14" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="29"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="25">
+        <v>0</v>
+      </c>
+      <c r="F46" s="47"/>
+      <c r="G46" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="33">
+        <v>16</v>
+      </c>
+      <c r="M46" s="33"/>
+      <c r="N46" s="33"/>
+    </row>
+    <row r="47" spans="1:14" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="31"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="25">
+        <v>0</v>
+      </c>
+      <c r="F47" s="47"/>
+      <c r="G47" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L47" s="34">
+        <f>SUM(L33:L46)/12</f>
+        <v>23</v>
+      </c>
+      <c r="M47" s="34">
+        <f>SUM(M33:M46)/12</f>
+        <v>38.416666666666664</v>
+      </c>
+      <c r="N47" s="34">
+        <f>SUM(N33:N46)/12</f>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24">
+        <v>4</v>
+      </c>
+      <c r="E48" s="25">
+        <v>7</v>
+      </c>
+      <c r="F48" s="47"/>
+      <c r="G48" s="27">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24">
         <v>1</v>
       </c>
-      <c r="E32" s="3">
-        <v>300</v>
-      </c>
-      <c r="F32" s="9">
-        <f t="shared" ref="F32:F38" si="2">D32*E32</f>
-        <v>300</v>
-      </c>
-      <c r="K32" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="L32" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="M32" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="44">
-        <v>30</v>
-      </c>
-      <c r="L33" s="44">
-        <v>32</v>
-      </c>
-      <c r="M33" s="44">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="44">
-        <v>30</v>
-      </c>
-      <c r="L34" s="44">
-        <v>32</v>
-      </c>
-      <c r="M34" s="44"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="44">
-        <v>30</v>
-      </c>
-      <c r="L35" s="44">
-        <v>65</v>
-      </c>
-      <c r="M35" s="44"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="44">
-        <v>30</v>
-      </c>
-      <c r="L36" s="44">
-        <v>65</v>
-      </c>
-      <c r="M36" s="44"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K37" s="44">
-        <v>30</v>
-      </c>
-      <c r="L37" s="44">
-        <v>73.5</v>
-      </c>
-      <c r="M37" s="44"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K38" s="44">
-        <v>30</v>
-      </c>
-      <c r="L38" s="44">
-        <v>73.5</v>
-      </c>
-      <c r="M38" s="44"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="10"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="13">
-        <f>D39*E39</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="44">
-        <v>8</v>
-      </c>
-      <c r="L39" s="44">
-        <v>120</v>
-      </c>
-      <c r="M39" s="44"/>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="24">
-        <f>SUM(F41:F54)</f>
-        <v>78</v>
-      </c>
-      <c r="K40" s="44">
-        <v>8</v>
-      </c>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="5">
-        <v>0</v>
-      </c>
-      <c r="E41" s="6">
-        <v>0</v>
-      </c>
-      <c r="F41" s="7">
-        <f>D41*E41</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="44">
-        <v>8</v>
-      </c>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
-    </row>
-    <row r="42" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="40" t="str">
-        <f>K32</f>
-        <v>2x2x 1/8</v>
-      </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="48">
-        <f>K47</f>
-        <v>23</v>
-      </c>
-      <c r="E42" s="31">
-        <v>0</v>
-      </c>
-      <c r="F42" s="33">
-        <f t="shared" ref="F42:F47" si="3">D42*E42</f>
-        <v>0</v>
-      </c>
-      <c r="K42" s="44">
-        <v>8</v>
-      </c>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-    </row>
-    <row r="43" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="40" t="str">
-        <f>L32</f>
-        <v>3x3x 1/8</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="48">
-        <f>L47</f>
-        <v>38.416666666666664</v>
-      </c>
-      <c r="E43" s="31">
-        <v>0</v>
-      </c>
-      <c r="F43" s="33">
+      <c r="E49" s="25">
+        <v>50</v>
+      </c>
+      <c r="F49" s="47"/>
+      <c r="G49" s="27">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K43" s="44">
-        <v>16</v>
-      </c>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-    </row>
-    <row r="44" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="40" t="str">
-        <f>M32</f>
-        <v>3x6x 1/8</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="48">
-        <f>M47</f>
-        <v>4.75</v>
-      </c>
-      <c r="E44" s="31">
-        <v>0</v>
-      </c>
-      <c r="F44" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="26"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K44" s="44">
-        <v>16</v>
-      </c>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-    </row>
-    <row r="45" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="31">
-        <v>0</v>
-      </c>
-      <c r="F45" s="33">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="26"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K45" s="44">
-        <v>16</v>
-      </c>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-    </row>
-    <row r="46" spans="1:13" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="38"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="31">
-        <v>0</v>
-      </c>
-      <c r="F46" s="33">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="26"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K46" s="45">
-        <v>16</v>
-      </c>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-    </row>
-    <row r="47" spans="1:13" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="40"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="31">
-        <v>0</v>
-      </c>
-      <c r="F47" s="33">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="26"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K47" s="46">
-        <f>SUM(K33:K46)/12</f>
-        <v>23</v>
-      </c>
-      <c r="L47" s="46">
-        <f>SUM(L33:L46)/12</f>
-        <v>38.416666666666664</v>
-      </c>
-      <c r="M47" s="46">
-        <f>SUM(M33:M46)/12</f>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2">
-        <v>4</v>
-      </c>
-      <c r="E48" s="3">
-        <v>7</v>
-      </c>
-      <c r="F48" s="9">
-        <f t="shared" ref="F48:F53" si="4">D48*E48</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3">
-        <v>50</v>
-      </c>
-      <c r="F49" s="9">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="8"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="10"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="13">
-        <f>D54*E54</f>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="10">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L30:N30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
@@ -2093,16 +2337,19 @@
     <hyperlink ref="C27" r:id="rId5" display="S50MST-A07P50P50 ()"/>
     <hyperlink ref="C15" r:id="rId6"/>
     <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="C6" r:id="rId8"/>
-    <hyperlink ref="C7" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C20" r:id="rId11"/>
-    <hyperlink ref="C23" r:id="rId12"/>
-    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="C7" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C20" r:id="rId10"/>
+    <hyperlink ref="C23" r:id="rId11"/>
+    <hyperlink ref="C8" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId13"/>
+    <hyperlink ref="C12" r:id="rId14"/>
+    <hyperlink ref="C24" r:id="rId15"/>
+    <hyperlink ref="C25" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
-  <drawing r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Found couplings for motor and pump. Unsure of pump keyway size, so got the larger option. Added Thumbs.db to the .gitignore file.
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -104,12 +104,6 @@
     <t>http://www.grainger.com/product/HALDEX-BARNES-Pump-4F651?s_pp=false</t>
   </si>
   <si>
-    <t>Coupling</t>
-  </si>
-  <si>
-    <t>S50MST-A07P50P50</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/CanaKit-Raspberry-Basic-Clear-Supply/dp/B00DG9D6IK/ref=sr_1_6?ie=UTF8&amp;qid=1390244948&amp;sr=8-6&amp;keywords=raspberry+pi</t>
   </si>
   <si>
@@ -122,24 +116,12 @@
     <t>https://www.sparkfun.com/products/312</t>
   </si>
   <si>
-    <t>Pressure Release</t>
-  </si>
-  <si>
-    <t>http://www.grainger.com/product/PRINCE-Relief-Valve-6X843?s_pp=false</t>
-  </si>
-  <si>
-    <t>Valve</t>
-  </si>
-  <si>
     <t>Tank</t>
   </si>
   <si>
     <t>http://www.northerntool.com/shop/tools/product_200466862_200466862</t>
   </si>
   <si>
-    <t>http://www.northerntool.com/shop/tools/product_200339057_200339057?cm_mmc=Google-pla-_-Hydraulics-_-Hydraulic%20Valves-_-201615&amp;ci_src=17588969&amp;ci_sku=201615&amp;gclid=COWNt4KIk7wCFahj7AodkDEA_g</t>
-  </si>
-  <si>
     <t>Better Valve</t>
   </si>
   <si>
@@ -155,15 +137,9 @@
     <t>Hydraulics</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
     <t>http://www.grainger.com/product/Spin-on-Filter-3KML8?s_pp=false</t>
   </si>
   <si>
-    <t>Filter Replacement</t>
-  </si>
-  <si>
     <t>http://www.grainger.com/product/PARKER-Filter-Element-1R412?opr=OAPD&amp;pbi=3KML8</t>
   </si>
   <si>
@@ -210,6 +186,39 @@
   </si>
   <si>
     <t>http://www.mcmaster.com/#9246k65/=qjbgg9</t>
+  </si>
+  <si>
+    <t>http://datasheets.maximintegrated.com/en/ds/MAX6955.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-Seg I2C </t>
+  </si>
+  <si>
+    <t>Tractor Supply</t>
+  </si>
+  <si>
+    <t>Filter housing</t>
+  </si>
+  <si>
+    <t>Filter Cartridge</t>
+  </si>
+  <si>
+    <t>Motor Coupling</t>
+  </si>
+  <si>
+    <t>Pump Coupling</t>
+  </si>
+  <si>
+    <t>Coupling Spider</t>
+  </si>
+  <si>
+    <t>http://www.amazonsupply.com/lovejoy-coupling-center-elastomer-spider/dp/B007SX3IO2/ref=sr_1_15?sr=1-15&amp;qid=1391886097</t>
+  </si>
+  <si>
+    <t>http://www.amazonsupply.com/lovejoy-standard-coupling-sintered-through/dp/B003HIWOGA/ref=sr_1_1_child?sr=1-1&amp;qid=1391886019</t>
+  </si>
+  <si>
+    <t>http://www.amazonsupply.com/s/ref=sp_search?guess=true&amp;Action=submit&amp;keywords=68514447952</t>
   </si>
 </sst>
 </file>
@@ -758,7 +767,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -823,6 +832,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -940,10 +950,10 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>485.45</c:v>
+                  <c:v>564.86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1742.07</c:v>
+                  <c:v>1676.1599999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>491.52</c:v>
@@ -996,7 +1006,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1308,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1349,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>5</v>
@@ -1352,17 +1362,17 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
       <c r="H3" s="20">
         <f>SUM(G4:G13)</f>
-        <v>485.45</v>
+        <v>564.86</v>
       </c>
       <c r="K3" s="6" t="str">
         <f>B3</f>
@@ -1370,7 +1380,7 @@
       </c>
       <c r="L3" s="17">
         <f>H3</f>
-        <v>485.45</v>
+        <v>564.86</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -1399,7 +1409,7 @@
       </c>
       <c r="L4" s="17">
         <f>H14</f>
-        <v>1742.07</v>
+        <v>1676.1599999999999</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1407,7 +1417,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="24">
         <v>1</v>
@@ -1419,7 +1429,7 @@
         <v>12.72</v>
       </c>
       <c r="G5" s="27">
-        <f t="shared" ref="G5:G12" si="0">(D5*E5)+F5</f>
+        <f t="shared" ref="G5:G13" si="0">(D5*E5)+F5</f>
         <v>67.72</v>
       </c>
       <c r="K5" s="6" t="str">
@@ -1436,7 +1446,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D6" s="24">
         <v>1</v>
@@ -1464,7 +1474,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" s="24">
         <v>1</v>
@@ -1484,7 +1494,7 @@
       </c>
       <c r="L7" s="22">
         <f>SUM(L3:L6)</f>
-        <v>3265.375</v>
+        <v>3278.875</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -1492,7 +1502,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D8" s="24">
         <v>1</v>
@@ -1519,7 +1529,9 @@
       <c r="E9" s="25">
         <v>5</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="41">
+        <v>0</v>
+      </c>
       <c r="G9" s="27">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1536,7 +1548,9 @@
       <c r="E10" s="25">
         <v>150</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="41">
+        <v>0</v>
+      </c>
       <c r="G10" s="27">
         <f t="shared" si="0"/>
         <v>150</v>
@@ -1544,10 +1558,10 @@
     </row>
     <row r="11" spans="2:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="24">
         <v>6</v>
@@ -1565,10 +1579,10 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D12" s="24">
         <v>1</v>
@@ -1585,28 +1599,38 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51">
-        <f>D13*E13</f>
-        <v>0</v>
+      <c r="B13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="48">
+        <v>3</v>
+      </c>
+      <c r="E13" s="49">
+        <v>23.97</v>
+      </c>
+      <c r="F13" s="50">
+        <v>7.5</v>
+      </c>
+      <c r="G13" s="27">
+        <f t="shared" si="0"/>
+        <v>79.41</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
+      <c r="B14" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="45">
         <f>SUM(G15:G29)</f>
-        <v>1742.07</v>
+        <v>1676.1599999999999</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -1643,7 +1667,9 @@
       <c r="E16" s="25">
         <v>123</v>
       </c>
-      <c r="F16" s="41"/>
+      <c r="F16" s="41">
+        <v>0</v>
+      </c>
       <c r="G16" s="27">
         <f t="shared" ref="G16:G28" si="1">(D16*E16)+F16</f>
         <v>123</v>
@@ -1672,7 +1698,7 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>15</v>
@@ -1683,7 +1709,9 @@
       <c r="E18" s="21">
         <v>391.5</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="41">
+        <v>0</v>
+      </c>
       <c r="G18" s="27">
         <f t="shared" si="1"/>
         <v>391.5</v>
@@ -1693,14 +1721,18 @@
       <c r="B19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="24" t="s">
+        <v>59</v>
+      </c>
       <c r="D19" s="24">
         <v>5</v>
       </c>
       <c r="E19" s="25">
         <v>100</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="41">
+        <v>0</v>
+      </c>
       <c r="G19" s="27">
         <f t="shared" si="1"/>
         <v>500</v>
@@ -1714,146 +1746,156 @@
         <v>36</v>
       </c>
       <c r="D20" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="25">
-        <v>78.5</v>
+        <v>85</v>
       </c>
       <c r="F20" s="41">
         <v>0</v>
       </c>
       <c r="G20" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D21" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="25">
-        <v>115</v>
-      </c>
-      <c r="F21" s="41"/>
+        <v>70</v>
+      </c>
+      <c r="F21" s="41">
+        <v>0</v>
+      </c>
       <c r="G21" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="24">
         <v>1</v>
       </c>
       <c r="E22" s="25">
-        <v>85</v>
-      </c>
-      <c r="F22" s="41"/>
+        <v>40</v>
+      </c>
+      <c r="F22" s="41">
+        <v>0</v>
+      </c>
       <c r="G22" s="27">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
       </c>
       <c r="E23" s="25">
-        <v>70</v>
-      </c>
-      <c r="F23" s="41"/>
+        <v>20</v>
+      </c>
+      <c r="F23" s="41">
+        <v>0</v>
+      </c>
       <c r="G23" s="27">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="25">
-        <v>40</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="26"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="41">
         <v>0</v>
       </c>
       <c r="G24" s="27">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>66</v>
       </c>
       <c r="D25" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="25">
-        <v>20</v>
+        <v>4.22</v>
       </c>
       <c r="F25" s="41">
         <v>0</v>
       </c>
       <c r="G25" s="27">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="26"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="41"/>
+      <c r="B26" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="24">
+        <v>1</v>
+      </c>
+      <c r="E26" s="25">
+        <v>5.29</v>
+      </c>
+      <c r="F26" s="41">
+        <v>0</v>
+      </c>
       <c r="G26" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+        <f>(D26*E26)+F26</f>
+        <v>5.29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D27" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" s="25">
-        <v>60</v>
-      </c>
-      <c r="F27" s="41"/>
+        <v>2.29</v>
+      </c>
+      <c r="F27" s="41">
+        <v>0</v>
+      </c>
       <c r="G27" s="27">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
@@ -1861,7 +1903,9 @@
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="25"/>
-      <c r="F28" s="41"/>
+      <c r="F28" s="41">
+        <v>0</v>
+      </c>
       <c r="G28" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1879,30 +1923,30 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
       <c r="H30" s="45">
         <f>SUM(G31:G39)</f>
         <v>491.52</v>
       </c>
-      <c r="L30" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="M30" s="61"/>
-      <c r="N30" s="62"/>
+      <c r="L30" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="M30" s="62"/>
+      <c r="N30" s="63"/>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="53" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D31" s="30">
         <v>4</v>
@@ -1910,16 +1954,18 @@
       <c r="E31" s="43">
         <v>47.88</v>
       </c>
-      <c r="F31" s="44"/>
+      <c r="F31" s="44">
+        <v>0</v>
+      </c>
       <c r="G31" s="47">
         <f>(D31*E31)+F31</f>
         <v>191.52</v>
       </c>
-      <c r="L31" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="M31" s="61"/>
-      <c r="N31" s="62"/>
+      <c r="L31" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" s="62"/>
+      <c r="N31" s="63"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="26" t="s">
@@ -1932,19 +1978,21 @@
       <c r="E32" s="25">
         <v>300</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="41">
+        <v>0</v>
+      </c>
       <c r="G32" s="27">
         <f t="shared" ref="G32:G39" si="2">(D32*E32)+F32</f>
         <v>300</v>
       </c>
       <c r="L32" s="35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M32" s="35" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="N32" s="35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -1952,7 +2000,9 @@
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="25"/>
-      <c r="F33" s="41"/>
+      <c r="F33" s="41">
+        <v>0</v>
+      </c>
       <c r="G33" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1972,7 +2022,9 @@
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="25"/>
-      <c r="F34" s="41"/>
+      <c r="F34" s="41">
+        <v>0</v>
+      </c>
       <c r="G34" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1990,7 +2042,9 @@
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="25"/>
-      <c r="F35" s="41"/>
+      <c r="F35" s="41">
+        <v>0</v>
+      </c>
       <c r="G35" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2008,7 +2062,9 @@
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="25"/>
-      <c r="F36" s="41"/>
+      <c r="F36" s="41">
+        <v>0</v>
+      </c>
       <c r="G36" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2026,7 +2082,9 @@
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="41"/>
+      <c r="F37" s="41">
+        <v>0</v>
+      </c>
       <c r="G37" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2044,7 +2102,9 @@
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="25"/>
-      <c r="F38" s="41"/>
+      <c r="F38" s="41">
+        <v>0</v>
+      </c>
       <c r="G38" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2062,7 +2122,9 @@
       <c r="C39" s="48"/>
       <c r="D39" s="48"/>
       <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
+      <c r="F39" s="50">
+        <v>0</v>
+      </c>
       <c r="G39" s="51">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2076,14 +2138,14 @@
       <c r="N39" s="32"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="60"/>
       <c r="H40" s="45">
         <f>SUM(G41:G54)</f>
         <v>546.33500000000004</v>
@@ -2099,7 +2161,7 @@
         <v>18</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D41" s="30">
         <v>0</v>
@@ -2107,7 +2169,9 @@
       <c r="E41" s="43">
         <v>0</v>
       </c>
-      <c r="F41" s="43"/>
+      <c r="F41" s="43">
+        <v>0</v>
+      </c>
       <c r="G41" s="47">
         <f>(E41*D41)+F41</f>
         <v>0</v>
@@ -2132,7 +2196,9 @@
         <f>56/24</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="F42" s="41"/>
+      <c r="F42" s="41">
+        <v>0</v>
+      </c>
       <c r="G42" s="27">
         <f>E42*D42</f>
         <v>53.666666666666671</v>
@@ -2157,7 +2223,9 @@
         <f>(87/24)</f>
         <v>3.625</v>
       </c>
-      <c r="F43" s="41"/>
+      <c r="F43" s="41">
+        <v>0</v>
+      </c>
       <c r="G43" s="27">
         <f t="shared" ref="G43:G44" si="3">E43*D43</f>
         <v>139.26041666666666</v>
@@ -2182,7 +2250,9 @@
         <f>193/24</f>
         <v>8.0416666666666661</v>
       </c>
-      <c r="F44" s="41"/>
+      <c r="F44" s="41">
+        <v>0</v>
+      </c>
       <c r="G44" s="27">
         <f t="shared" si="3"/>
         <v>38.197916666666664</v>
@@ -2195,10 +2265,10 @@
     </row>
     <row r="45" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="30">
@@ -2207,7 +2277,9 @@
       <c r="E45" s="25">
         <v>10</v>
       </c>
-      <c r="F45" s="41"/>
+      <c r="F45" s="41">
+        <v>0</v>
+      </c>
       <c r="G45" s="27">
         <f>D45*E45</f>
         <v>60</v>
@@ -2225,7 +2297,9 @@
       <c r="E46" s="25">
         <v>0</v>
       </c>
-      <c r="F46" s="41"/>
+      <c r="F46" s="41">
+        <v>0</v>
+      </c>
       <c r="G46" s="27">
         <f t="shared" ref="G46:G54" si="4">(E46*D46)+F46</f>
         <v>0</v>
@@ -2243,7 +2317,9 @@
       <c r="E47" s="25">
         <v>0</v>
       </c>
-      <c r="F47" s="41"/>
+      <c r="F47" s="41">
+        <v>0</v>
+      </c>
       <c r="G47" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2272,7 +2348,9 @@
       <c r="E48" s="25">
         <v>7</v>
       </c>
-      <c r="F48" s="41"/>
+      <c r="F48" s="41">
+        <v>0</v>
+      </c>
       <c r="G48" s="27">
         <f t="shared" si="4"/>
         <v>70</v>
@@ -2280,10 +2358,10 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="26" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D49" s="24">
         <v>1</v>
@@ -2291,7 +2369,9 @@
       <c r="E49" s="25">
         <v>185.21</v>
       </c>
-      <c r="F49" s="41"/>
+      <c r="F49" s="41">
+        <v>0</v>
+      </c>
       <c r="G49" s="27">
         <f t="shared" si="4"/>
         <v>185.21</v>
@@ -2302,7 +2382,9 @@
       <c r="C50" s="24"/>
       <c r="D50" s="24"/>
       <c r="E50" s="25"/>
-      <c r="F50" s="41"/>
+      <c r="F50" s="41">
+        <v>0</v>
+      </c>
       <c r="G50" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2313,7 +2395,9 @@
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
       <c r="E51" s="25"/>
-      <c r="F51" s="41"/>
+      <c r="F51" s="41">
+        <v>0</v>
+      </c>
       <c r="G51" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2324,7 +2408,9 @@
       <c r="C52" s="24"/>
       <c r="D52" s="24"/>
       <c r="E52" s="25"/>
-      <c r="F52" s="41"/>
+      <c r="F52" s="41">
+        <v>0</v>
+      </c>
       <c r="G52" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2335,7 +2421,9 @@
       <c r="C53" s="24"/>
       <c r="D53" s="24"/>
       <c r="E53" s="25"/>
-      <c r="F53" s="41"/>
+      <c r="F53" s="41">
+        <v>0</v>
+      </c>
       <c r="G53" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2346,7 +2434,9 @@
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="9"/>
-      <c r="F54" s="42"/>
+      <c r="F54" s="42">
+        <v>0</v>
+      </c>
       <c r="G54" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2366,20 +2456,20 @@
     <hyperlink ref="C17" r:id="rId2"/>
     <hyperlink ref="C18" r:id="rId3"/>
     <hyperlink ref="C16" r:id="rId4"/>
-    <hyperlink ref="C27" r:id="rId5" display="S50MST-A07P50P50 ()"/>
-    <hyperlink ref="C15" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="C7" r:id="rId8"/>
-    <hyperlink ref="C11" r:id="rId9"/>
-    <hyperlink ref="C20" r:id="rId10"/>
-    <hyperlink ref="C23" r:id="rId11"/>
-    <hyperlink ref="C8" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="C12" r:id="rId14"/>
-    <hyperlink ref="C24" r:id="rId15"/>
-    <hyperlink ref="C25" r:id="rId16"/>
-    <hyperlink ref="C31" r:id="rId17" location="22665t31/=qjbaja" display="http://www.mcmaster.com/ - 22665t31/=qjbaja"/>
-    <hyperlink ref="C49" r:id="rId18" location="9246k65/=qjbgg9"/>
+    <hyperlink ref="C15" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="C21" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="C6" r:id="rId11"/>
+    <hyperlink ref="C12" r:id="rId12"/>
+    <hyperlink ref="C22" r:id="rId13"/>
+    <hyperlink ref="C23" r:id="rId14"/>
+    <hyperlink ref="C31" r:id="rId15" location="22665t31/=qjbaja" display="http://www.mcmaster.com/ - 22665t31/=qjbaja"/>
+    <hyperlink ref="C49" r:id="rId16" location="9246k65/=qjbgg9"/>
+    <hyperlink ref="C13" r:id="rId17"/>
+    <hyperlink ref="C25" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
Made a page on the BOM for the presentation. (Removed links and shrunk the page) Presentation is done except for the electrical slide.
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="10515" windowHeight="7875"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="10515" windowHeight="7875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Mike" sheetId="6" r:id="rId3"/>
     <sheet name="Geoff" sheetId="7" r:id="rId4"/>
     <sheet name="TBD" sheetId="8" r:id="rId5"/>
+    <sheet name="Presentation Budget" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bob!$A$1:$I$140</definedName>
@@ -261,11 +262,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#.0\ &quot;in&quot;"/>
     <numFmt numFmtId="165" formatCode="#.00\ &quot;ft&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -315,7 +317,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -869,13 +871,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -979,6 +999,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1437,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35627,4 +35676,2405 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K159"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="73" t="str">
+        <f>Main!B2</f>
+        <v>Name</v>
+      </c>
+      <c r="B2" s="81" t="str">
+        <f>Main!E2</f>
+        <v>Qt</v>
+      </c>
+      <c r="C2" s="81" t="str">
+        <f>Main!F2</f>
+        <v xml:space="preserve">Price </v>
+      </c>
+      <c r="D2" s="81" t="str">
+        <f>Main!G2</f>
+        <v>Shipping</v>
+      </c>
+      <c r="E2" s="74" t="str">
+        <f>Main!H2</f>
+        <v>Total</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="2" t="str">
+        <f>Main!L2</f>
+        <v>Category</v>
+      </c>
+      <c r="J2" s="16" t="str">
+        <f>Main!M2</f>
+        <v>Total</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="82" t="str">
+        <f>Main!B3</f>
+        <v>Electronics</v>
+      </c>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="88">
+        <f>Main!I3</f>
+        <v>600.94999999999993</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="26" t="str">
+        <f>Main!L3</f>
+        <v>Electronics</v>
+      </c>
+      <c r="J3" s="76">
+        <f>Main!M3</f>
+        <v>600.94999999999993</v>
+      </c>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="str">
+        <f>Main!B4</f>
+        <v>7 segment display</v>
+      </c>
+      <c r="B4" s="3">
+        <f>Main!E4</f>
+        <v>5</v>
+      </c>
+      <c r="C4" s="85">
+        <f>Main!F4</f>
+        <v>16.46</v>
+      </c>
+      <c r="D4" s="85">
+        <f>Main!G4</f>
+        <v>15</v>
+      </c>
+      <c r="E4" s="86">
+        <f>Main!H4</f>
+        <v>97.300000000000011</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="26" t="str">
+        <f>Main!L4</f>
+        <v>Hydraulics</v>
+      </c>
+      <c r="J4" s="76">
+        <f>Main!M4</f>
+        <v>1676.1599999999999</v>
+      </c>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="str">
+        <f>Main!B5</f>
+        <v>Rasberry Pi</v>
+      </c>
+      <c r="B5" s="24">
+        <f>Main!E5</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="87">
+        <f>Main!F5</f>
+        <v>55</v>
+      </c>
+      <c r="D5" s="87">
+        <f>Main!G5</f>
+        <v>12.72</v>
+      </c>
+      <c r="E5" s="76">
+        <f>Main!H5</f>
+        <v>67.72</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="26" t="str">
+        <f>Main!L5</f>
+        <v>Mechanical</v>
+      </c>
+      <c r="J5" s="76">
+        <f>Main!M5</f>
+        <v>491.52</v>
+      </c>
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="str">
+        <f>Main!B6</f>
+        <v>Monitor</v>
+      </c>
+      <c r="B6" s="24">
+        <f>Main!E6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="87">
+        <f>Main!F6</f>
+        <v>136</v>
+      </c>
+      <c r="D6" s="87">
+        <f>Main!G6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="76">
+        <f>Main!H6</f>
+        <v>136</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="26" t="str">
+        <f>Main!L6</f>
+        <v>Raw Materials</v>
+      </c>
+      <c r="J6" s="76">
+        <f>Main!M6</f>
+        <v>565.43395833333329</v>
+      </c>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="str">
+        <f>Main!B7</f>
+        <v>hdmi cord</v>
+      </c>
+      <c r="B7" s="24">
+        <f>Main!E7</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="87">
+        <f>Main!F7</f>
+        <v>5.79</v>
+      </c>
+      <c r="D7" s="87">
+        <f>Main!G7</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="76">
+        <f>Main!H7</f>
+        <v>5.79</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="75" t="str">
+        <f>Main!L7</f>
+        <v>Total</v>
+      </c>
+      <c r="J7" s="77">
+        <f>Main!M7</f>
+        <v>3334.0639583333332</v>
+      </c>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="str">
+        <f>Main!B8</f>
+        <v>i2c ADC</v>
+      </c>
+      <c r="B8" s="24">
+        <f>Main!E8</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="87">
+        <f>Main!F8</f>
+        <v>14.95</v>
+      </c>
+      <c r="D8" s="87">
+        <f>Main!G8</f>
+        <v>4.07</v>
+      </c>
+      <c r="E8" s="76">
+        <f>Main!H8</f>
+        <v>19.02</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="str">
+        <f>Main!B9</f>
+        <v>Switches</v>
+      </c>
+      <c r="B9" s="24">
+        <f>Main!E9</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="87">
+        <f>Main!F9</f>
+        <v>5.95</v>
+      </c>
+      <c r="D9" s="87">
+        <f>Main!G9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="76">
+        <f>Main!H9</f>
+        <v>5.95</v>
+      </c>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="str">
+        <f>Main!B10</f>
+        <v xml:space="preserve">Misc </v>
+      </c>
+      <c r="B10" s="24">
+        <f>Main!E10</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="87">
+        <f>Main!F10</f>
+        <v>150</v>
+      </c>
+      <c r="D10" s="87">
+        <f>Main!G10</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="76">
+        <f>Main!H10</f>
+        <v>150</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="str">
+        <f>Main!B11</f>
+        <v>Darlington Array</v>
+      </c>
+      <c r="B11" s="24">
+        <f>Main!E11</f>
+        <v>6</v>
+      </c>
+      <c r="C11" s="87">
+        <f>Main!F11</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="87">
+        <f>Main!G11</f>
+        <v>4.43</v>
+      </c>
+      <c r="E11" s="76">
+        <f>Main!H11</f>
+        <v>16.43</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="str">
+        <f>Main!B12</f>
+        <v>USB external HDD</v>
+      </c>
+      <c r="B12" s="24">
+        <f>Main!E12</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="87">
+        <f>Main!F12</f>
+        <v>28</v>
+      </c>
+      <c r="D12" s="87">
+        <f>Main!G12</f>
+        <v>7.49</v>
+      </c>
+      <c r="E12" s="76">
+        <f>Main!H12</f>
+        <v>35.49</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="str">
+        <f>Main!B13</f>
+        <v xml:space="preserve">7-Seg I2C </v>
+      </c>
+      <c r="B13" s="24">
+        <f>Main!E13</f>
+        <v>5</v>
+      </c>
+      <c r="C13" s="87">
+        <f>Main!F13</f>
+        <v>5.95</v>
+      </c>
+      <c r="D13" s="87">
+        <f>Main!G13</f>
+        <v>7.5</v>
+      </c>
+      <c r="E13" s="76">
+        <f>Main!H13</f>
+        <v>37.25</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="str">
+        <f>Main!B14</f>
+        <v>Wireless router</v>
+      </c>
+      <c r="B14" s="24">
+        <f>Main!E14</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="87">
+        <f>Main!F14</f>
+        <v>30</v>
+      </c>
+      <c r="D14" s="87">
+        <f>Main!G14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="76">
+        <f>Main!H14</f>
+        <v>30</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="83" t="str">
+        <f>Main!B17</f>
+        <v>Hydraulics</v>
+      </c>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="88">
+        <f>Main!I17</f>
+        <v>1676.1599999999999</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="str">
+        <f>Main!B18</f>
+        <v>Pump</v>
+      </c>
+      <c r="B16" s="3">
+        <f>Main!E18</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="87">
+        <f>Main!F18</f>
+        <v>171.75</v>
+      </c>
+      <c r="D16" s="87">
+        <f>Main!G18</f>
+        <v>24.32</v>
+      </c>
+      <c r="E16" s="87">
+        <f>Main!H18</f>
+        <v>196.07</v>
+      </c>
+      <c r="F16" s="89"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="str">
+        <f>Main!B19</f>
+        <v>Motor</v>
+      </c>
+      <c r="B17" s="24">
+        <f>Main!E19</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="87">
+        <f>Main!F19</f>
+        <v>123</v>
+      </c>
+      <c r="D17" s="87">
+        <f>Main!G19</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="87">
+        <f>Main!H19</f>
+        <v>123</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="str">
+        <f>Main!B20</f>
+        <v>Cylinder</v>
+      </c>
+      <c r="B18" s="24">
+        <f>Main!E20</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="87">
+        <f>Main!F20</f>
+        <v>236.5</v>
+      </c>
+      <c r="D18" s="87">
+        <f>Main!G20</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="87">
+        <f>Main!H20</f>
+        <v>236.5</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="str">
+        <f>Main!B21</f>
+        <v>Sensor (0-5V)</v>
+      </c>
+      <c r="B19" s="24">
+        <f>Main!E21</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="87">
+        <f>Main!F21</f>
+        <v>391.5</v>
+      </c>
+      <c r="D19" s="87">
+        <f>Main!G21</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="87">
+        <f>Main!H21</f>
+        <v>391.5</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="str">
+        <f>Main!B22</f>
+        <v>Lines</v>
+      </c>
+      <c r="B20" s="24">
+        <f>Main!E22</f>
+        <v>5</v>
+      </c>
+      <c r="C20" s="87">
+        <f>Main!F22</f>
+        <v>100</v>
+      </c>
+      <c r="D20" s="87">
+        <f>Main!G22</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="87">
+        <f>Main!H22</f>
+        <v>500</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="str">
+        <f>Main!B23</f>
+        <v>Valve</v>
+      </c>
+      <c r="B21" s="24">
+        <f>Main!E23</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="87">
+        <f>Main!F23</f>
+        <v>85</v>
+      </c>
+      <c r="D21" s="87">
+        <f>Main!G23</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="87">
+        <f>Main!H23</f>
+        <v>85</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="str">
+        <f>Main!B24</f>
+        <v>Tank</v>
+      </c>
+      <c r="B22" s="24">
+        <f>Main!E24</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="87">
+        <f>Main!F24</f>
+        <v>70</v>
+      </c>
+      <c r="D22" s="87">
+        <f>Main!G24</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="87">
+        <f>Main!H24</f>
+        <v>70</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="str">
+        <f>Main!B25</f>
+        <v>Filter housing</v>
+      </c>
+      <c r="B23" s="24">
+        <f>Main!E25</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="87">
+        <f>Main!F25</f>
+        <v>40</v>
+      </c>
+      <c r="D23" s="87">
+        <f>Main!G25</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="87">
+        <f>Main!H25</f>
+        <v>40</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="str">
+        <f>Main!B26</f>
+        <v>Filter Cartridge</v>
+      </c>
+      <c r="B24" s="24">
+        <f>Main!E26</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="87">
+        <f>Main!F26</f>
+        <v>20</v>
+      </c>
+      <c r="D24" s="87">
+        <f>Main!G26</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="87">
+        <f>Main!H26</f>
+        <v>20</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
+        <f>Main!B27</f>
+        <v>0</v>
+      </c>
+      <c r="B25" s="24">
+        <f>Main!E27</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="87">
+        <f>Main!F27</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="87">
+        <f>Main!G27</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="87">
+        <f>Main!H27</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="str">
+        <f>Main!B28</f>
+        <v>Motor Coupling</v>
+      </c>
+      <c r="B26" s="24">
+        <f>Main!E28</f>
+        <v>1</v>
+      </c>
+      <c r="C26" s="87">
+        <f>Main!F28</f>
+        <v>4.22</v>
+      </c>
+      <c r="D26" s="87">
+        <f>Main!G28</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="87">
+        <f>Main!H28</f>
+        <v>4.22</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="str">
+        <f>Main!B29</f>
+        <v>Pump Coupling</v>
+      </c>
+      <c r="B27" s="24">
+        <f>Main!E29</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="87">
+        <f>Main!F29</f>
+        <v>5.29</v>
+      </c>
+      <c r="D27" s="87">
+        <f>Main!G29</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="87">
+        <f>Main!H29</f>
+        <v>5.29</v>
+      </c>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="26" t="str">
+        <f>Main!B30</f>
+        <v>Coupling Spider</v>
+      </c>
+      <c r="B28" s="24">
+        <f>Main!E30</f>
+        <v>2</v>
+      </c>
+      <c r="C28" s="87">
+        <f>Main!F30</f>
+        <v>2.29</v>
+      </c>
+      <c r="D28" s="87">
+        <f>Main!G30</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="87">
+        <f>Main!H30</f>
+        <v>4.58</v>
+      </c>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="83" t="str">
+        <f>Main!B33</f>
+        <v>Mechanical</v>
+      </c>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="88">
+        <f>Main!I33</f>
+        <v>491.52</v>
+      </c>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="str">
+        <f>Main!B34</f>
+        <v>Castors</v>
+      </c>
+      <c r="B30" s="3">
+        <f>Main!E34</f>
+        <v>4</v>
+      </c>
+      <c r="C30" s="87">
+        <f>Main!F34</f>
+        <v>47.88</v>
+      </c>
+      <c r="D30" s="87">
+        <f>Main!G34</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="87">
+        <f>Main!H34</f>
+        <v>191.52</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="str">
+        <f>Main!B35</f>
+        <v>Misc Hardware</v>
+      </c>
+      <c r="B31" s="24">
+        <f>Main!E35</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="87">
+        <f>Main!F35</f>
+        <v>300</v>
+      </c>
+      <c r="D31" s="87">
+        <f>Main!G35</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="87">
+        <f>Main!H35</f>
+        <v>300</v>
+      </c>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="83" t="str">
+        <f>Main!B43</f>
+        <v>Raw Materials</v>
+      </c>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="88">
+        <f>Main!I43</f>
+        <v>565.43395833333329</v>
+      </c>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="str">
+        <f>Main!B44</f>
+        <v>Frame Steel</v>
+      </c>
+      <c r="B33" s="3">
+        <f>Main!E44</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="87">
+        <f>Main!F44</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="87">
+        <f>Main!G44</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="87">
+        <f>Main!H44</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="str">
+        <f>Main!B45</f>
+        <v>2x2x 1/8</v>
+      </c>
+      <c r="B34" s="24">
+        <f>Main!E45</f>
+        <v>23</v>
+      </c>
+      <c r="C34" s="87">
+        <f>Main!F45</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="D34" s="87">
+        <f>Main!G45</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="87">
+        <f>Main!H45</f>
+        <v>53.666666666666671</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="str">
+        <f>Main!B46</f>
+        <v>3x3x 1/8</v>
+      </c>
+      <c r="B35" s="24">
+        <f>Main!E46</f>
+        <v>38.416666666666664</v>
+      </c>
+      <c r="C35" s="87">
+        <f>Main!F46</f>
+        <v>3.625</v>
+      </c>
+      <c r="D35" s="87">
+        <f>Main!G46</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="87">
+        <f>Main!H46</f>
+        <v>139.26041666666666</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="str">
+        <f>Main!B47</f>
+        <v>3x6x 3/16</v>
+      </c>
+      <c r="B36" s="24">
+        <f>Main!E47</f>
+        <v>4.75</v>
+      </c>
+      <c r="C36" s="87">
+        <f>Main!F47</f>
+        <v>12.0625</v>
+      </c>
+      <c r="D36" s="87">
+        <f>Main!G47</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="87">
+        <f>Main!H47</f>
+        <v>57.296875</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="str">
+        <f>Main!B48</f>
+        <v>Steel Cuts at Capitol</v>
+      </c>
+      <c r="B37" s="24">
+        <f>Main!E48</f>
+        <v>6</v>
+      </c>
+      <c r="C37" s="87">
+        <f>Main!F48</f>
+        <v>10</v>
+      </c>
+      <c r="D37" s="87">
+        <f>Main!G48</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="87">
+        <f>Main!H48</f>
+        <v>60</v>
+      </c>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="26">
+        <f>Main!B49</f>
+        <v>0</v>
+      </c>
+      <c r="B38" s="24">
+        <f>Main!E49</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="87">
+        <f>Main!F49</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="87">
+        <f>Main!G49</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="87">
+        <f>Main!H49</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="26">
+        <f>Main!B50</f>
+        <v>0</v>
+      </c>
+      <c r="B39" s="24">
+        <f>Main!E50</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="87">
+        <f>Main!F50</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="87">
+        <f>Main!G50</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="87">
+        <f>Main!H50</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="str">
+        <f>Main!B51</f>
+        <v>Paint</v>
+      </c>
+      <c r="B40" s="24">
+        <f>Main!E51</f>
+        <v>10</v>
+      </c>
+      <c r="C40" s="87">
+        <f>Main!F51</f>
+        <v>7</v>
+      </c>
+      <c r="D40" s="87">
+        <f>Main!G51</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="87">
+        <f>Main!H51</f>
+        <v>70</v>
+      </c>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="str">
+        <f>Main!B52</f>
+        <v>Aluminum plate 1'x6'x.5"</v>
+      </c>
+      <c r="B41" s="8">
+        <f>Main!E52</f>
+        <v>1</v>
+      </c>
+      <c r="C41" s="87">
+        <f>Main!F52</f>
+        <v>185.21</v>
+      </c>
+      <c r="D41" s="87">
+        <f>Main!G52</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="87">
+        <f>Main!H52</f>
+        <v>185.21</v>
+      </c>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="23"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="23"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="23"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="23"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="23"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="23"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="23"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="23"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
+      <c r="H79" s="23"/>
+      <c r="I79" s="23"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="23"/>
+      <c r="I81" s="23"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="23"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="23"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="23"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="23"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="23"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="23"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="23"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="23"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="23"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="23"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="23"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="23"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="23"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23"/>
+      <c r="I92" s="23"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="23"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="23"/>
+      <c r="I93" s="23"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="23"/>
+      <c r="B94" s="23"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="23"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="23"/>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="23"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="23"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="23"/>
+      <c r="I96" s="23"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="23"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="23"/>
+      <c r="I97" s="23"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="23"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="23"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
+      <c r="H98" s="23"/>
+      <c r="I98" s="23"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="23"/>
+      <c r="B99" s="23"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
+      <c r="H99" s="23"/>
+      <c r="I99" s="23"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="23"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
+      <c r="H100" s="23"/>
+      <c r="I100" s="23"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="23"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="23"/>
+      <c r="H101" s="23"/>
+      <c r="I101" s="23"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="23"/>
+      <c r="B102" s="23"/>
+      <c r="C102" s="23"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="23"/>
+      <c r="H102" s="23"/>
+      <c r="I102" s="23"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="23"/>
+      <c r="B103" s="23"/>
+      <c r="C103" s="23"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="23"/>
+      <c r="H103" s="23"/>
+      <c r="I103" s="23"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="23"/>
+      <c r="B104" s="23"/>
+      <c r="C104" s="23"/>
+      <c r="D104" s="23"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="23"/>
+      <c r="I104" s="23"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="23"/>
+      <c r="B105" s="23"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="23"/>
+      <c r="H105" s="23"/>
+      <c r="I105" s="23"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="23"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="23"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
+      <c r="H106" s="23"/>
+      <c r="I106" s="23"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="23"/>
+      <c r="B107" s="23"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="23"/>
+      <c r="H107" s="23"/>
+      <c r="I107" s="23"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="23"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="23"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23"/>
+      <c r="H108" s="23"/>
+      <c r="I108" s="23"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="23"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="23"/>
+      <c r="I109" s="23"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="23"/>
+      <c r="B110" s="23"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23"/>
+      <c r="H110" s="23"/>
+      <c r="I110" s="23"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="23"/>
+      <c r="B111" s="23"/>
+      <c r="C111" s="23"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="23"/>
+      <c r="H111" s="23"/>
+      <c r="I111" s="23"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="23"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="23"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="23"/>
+      <c r="H112" s="23"/>
+      <c r="I112" s="23"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="23"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="23"/>
+      <c r="H113" s="23"/>
+      <c r="I113" s="23"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="23"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
+      <c r="H114" s="23"/>
+      <c r="I114" s="23"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="23"/>
+      <c r="B115" s="23"/>
+      <c r="C115" s="23"/>
+      <c r="D115" s="23"/>
+      <c r="E115" s="23"/>
+      <c r="F115" s="23"/>
+      <c r="G115" s="23"/>
+      <c r="H115" s="23"/>
+      <c r="I115" s="23"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="23"/>
+      <c r="B116" s="23"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="23"/>
+      <c r="E116" s="23"/>
+      <c r="F116" s="23"/>
+      <c r="G116" s="23"/>
+      <c r="H116" s="23"/>
+      <c r="I116" s="23"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="23"/>
+      <c r="B117" s="23"/>
+      <c r="C117" s="23"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="23"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="23"/>
+      <c r="I117" s="23"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="23"/>
+      <c r="B118" s="23"/>
+      <c r="C118" s="23"/>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="23"/>
+      <c r="H118" s="23"/>
+      <c r="I118" s="23"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="23"/>
+      <c r="B119" s="23"/>
+      <c r="C119" s="23"/>
+      <c r="D119" s="23"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="23"/>
+      <c r="G119" s="23"/>
+      <c r="H119" s="23"/>
+      <c r="I119" s="23"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="23"/>
+      <c r="B120" s="23"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="23"/>
+      <c r="F120" s="23"/>
+      <c r="G120" s="23"/>
+      <c r="H120" s="23"/>
+      <c r="I120" s="23"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="23"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="23"/>
+      <c r="H121" s="23"/>
+      <c r="I121" s="23"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="23"/>
+      <c r="B122" s="23"/>
+      <c r="C122" s="23"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="23"/>
+      <c r="H122" s="23"/>
+      <c r="I122" s="23"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="23"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="23"/>
+      <c r="F123" s="23"/>
+      <c r="G123" s="23"/>
+      <c r="H123" s="23"/>
+      <c r="I123" s="23"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="23"/>
+      <c r="B124" s="23"/>
+      <c r="C124" s="23"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="23"/>
+      <c r="H124" s="23"/>
+      <c r="I124" s="23"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="23"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="23"/>
+      <c r="G125" s="23"/>
+      <c r="H125" s="23"/>
+      <c r="I125" s="23"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="23"/>
+      <c r="B126" s="23"/>
+      <c r="C126" s="23"/>
+      <c r="D126" s="23"/>
+      <c r="E126" s="23"/>
+      <c r="F126" s="23"/>
+      <c r="G126" s="23"/>
+      <c r="H126" s="23"/>
+      <c r="I126" s="23"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="23"/>
+      <c r="B127" s="23"/>
+      <c r="C127" s="23"/>
+      <c r="D127" s="23"/>
+      <c r="E127" s="23"/>
+      <c r="F127" s="23"/>
+      <c r="G127" s="23"/>
+      <c r="H127" s="23"/>
+      <c r="I127" s="23"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="23"/>
+      <c r="B128" s="23"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="23"/>
+      <c r="G128" s="23"/>
+      <c r="H128" s="23"/>
+      <c r="I128" s="23"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="23"/>
+      <c r="B129" s="23"/>
+      <c r="C129" s="23"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="23"/>
+      <c r="F129" s="23"/>
+      <c r="G129" s="23"/>
+      <c r="H129" s="23"/>
+      <c r="I129" s="23"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="23"/>
+      <c r="B130" s="23"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23"/>
+      <c r="F130" s="23"/>
+      <c r="G130" s="23"/>
+      <c r="H130" s="23"/>
+      <c r="I130" s="23"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="23"/>
+      <c r="B131" s="23"/>
+      <c r="C131" s="23"/>
+      <c r="D131" s="23"/>
+      <c r="E131" s="23"/>
+      <c r="F131" s="23"/>
+      <c r="G131" s="23"/>
+      <c r="H131" s="23"/>
+      <c r="I131" s="23"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="23"/>
+      <c r="B132" s="23"/>
+      <c r="C132" s="23"/>
+      <c r="D132" s="23"/>
+      <c r="E132" s="23"/>
+      <c r="F132" s="23"/>
+      <c r="G132" s="23"/>
+      <c r="H132" s="23"/>
+      <c r="I132" s="23"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="23"/>
+      <c r="B133" s="23"/>
+      <c r="C133" s="23"/>
+      <c r="D133" s="23"/>
+      <c r="E133" s="23"/>
+      <c r="F133" s="23"/>
+      <c r="G133" s="23"/>
+      <c r="H133" s="23"/>
+      <c r="I133" s="23"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="23"/>
+      <c r="B134" s="23"/>
+      <c r="C134" s="23"/>
+      <c r="D134" s="23"/>
+      <c r="E134" s="23"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="23"/>
+      <c r="H134" s="23"/>
+      <c r="I134" s="23"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="23"/>
+      <c r="B135" s="23"/>
+      <c r="C135" s="23"/>
+      <c r="D135" s="23"/>
+      <c r="E135" s="23"/>
+      <c r="F135" s="23"/>
+      <c r="G135" s="23"/>
+      <c r="H135" s="23"/>
+      <c r="I135" s="23"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="23"/>
+      <c r="B136" s="23"/>
+      <c r="C136" s="23"/>
+      <c r="D136" s="23"/>
+      <c r="E136" s="23"/>
+      <c r="F136" s="23"/>
+      <c r="G136" s="23"/>
+      <c r="H136" s="23"/>
+      <c r="I136" s="23"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="23"/>
+      <c r="B137" s="23"/>
+      <c r="C137" s="23"/>
+      <c r="D137" s="23"/>
+      <c r="E137" s="23"/>
+      <c r="F137" s="23"/>
+      <c r="G137" s="23"/>
+      <c r="H137" s="23"/>
+      <c r="I137" s="23"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="23"/>
+      <c r="B138" s="23"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="23"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="23"/>
+      <c r="G138" s="23"/>
+      <c r="H138" s="23"/>
+      <c r="I138" s="23"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="23"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
+      <c r="D139" s="23"/>
+      <c r="E139" s="23"/>
+      <c r="F139" s="23"/>
+      <c r="G139" s="23"/>
+      <c r="H139" s="23"/>
+      <c r="I139" s="23"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="23"/>
+      <c r="B140" s="23"/>
+      <c r="C140" s="23"/>
+      <c r="D140" s="23"/>
+      <c r="E140" s="23"/>
+      <c r="F140" s="23"/>
+      <c r="G140" s="23"/>
+      <c r="H140" s="23"/>
+      <c r="I140" s="23"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="23"/>
+      <c r="B141" s="23"/>
+      <c r="C141" s="23"/>
+      <c r="D141" s="23"/>
+      <c r="E141" s="23"/>
+      <c r="F141" s="23"/>
+      <c r="G141" s="23"/>
+      <c r="H141" s="23"/>
+      <c r="I141" s="23"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="23"/>
+      <c r="B142" s="23"/>
+      <c r="C142" s="23"/>
+      <c r="D142" s="23"/>
+      <c r="E142" s="23"/>
+      <c r="F142" s="23"/>
+      <c r="G142" s="23"/>
+      <c r="H142" s="23"/>
+      <c r="I142" s="23"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="23"/>
+      <c r="B143" s="23"/>
+      <c r="C143" s="23"/>
+      <c r="D143" s="23"/>
+      <c r="E143" s="23"/>
+      <c r="F143" s="23"/>
+      <c r="G143" s="23"/>
+      <c r="H143" s="23"/>
+      <c r="I143" s="23"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="23"/>
+      <c r="B144" s="23"/>
+      <c r="C144" s="23"/>
+      <c r="D144" s="23"/>
+      <c r="E144" s="23"/>
+      <c r="F144" s="23"/>
+      <c r="G144" s="23"/>
+      <c r="H144" s="23"/>
+      <c r="I144" s="23"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="23"/>
+      <c r="B145" s="23"/>
+      <c r="C145" s="23"/>
+      <c r="D145" s="23"/>
+      <c r="E145" s="23"/>
+      <c r="F145" s="23"/>
+      <c r="G145" s="23"/>
+      <c r="H145" s="23"/>
+      <c r="I145" s="23"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="23"/>
+      <c r="B146" s="23"/>
+      <c r="C146" s="23"/>
+      <c r="D146" s="23"/>
+      <c r="E146" s="23"/>
+      <c r="F146" s="23"/>
+      <c r="G146" s="23"/>
+      <c r="H146" s="23"/>
+      <c r="I146" s="23"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="23"/>
+      <c r="B147" s="23"/>
+      <c r="C147" s="23"/>
+      <c r="D147" s="23"/>
+      <c r="E147" s="23"/>
+      <c r="F147" s="23"/>
+      <c r="G147" s="23"/>
+      <c r="H147" s="23"/>
+      <c r="I147" s="23"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="23"/>
+      <c r="B148" s="23"/>
+      <c r="C148" s="23"/>
+      <c r="D148" s="23"/>
+      <c r="E148" s="23"/>
+      <c r="F148" s="23"/>
+      <c r="G148" s="23"/>
+      <c r="H148" s="23"/>
+      <c r="I148" s="23"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="23"/>
+      <c r="B149" s="23"/>
+      <c r="C149" s="23"/>
+      <c r="D149" s="23"/>
+      <c r="E149" s="23"/>
+      <c r="F149" s="23"/>
+      <c r="G149" s="23"/>
+      <c r="H149" s="23"/>
+      <c r="I149" s="23"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="23"/>
+      <c r="B150" s="23"/>
+      <c r="C150" s="23"/>
+      <c r="D150" s="23"/>
+      <c r="E150" s="23"/>
+      <c r="F150" s="23"/>
+      <c r="G150" s="23"/>
+      <c r="H150" s="23"/>
+      <c r="I150" s="23"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="23"/>
+      <c r="B151" s="23"/>
+      <c r="C151" s="23"/>
+      <c r="D151" s="23"/>
+      <c r="E151" s="23"/>
+      <c r="F151" s="23"/>
+      <c r="G151" s="23"/>
+      <c r="H151" s="23"/>
+      <c r="I151" s="23"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="23"/>
+      <c r="B152" s="23"/>
+      <c r="C152" s="23"/>
+      <c r="D152" s="23"/>
+      <c r="E152" s="23"/>
+      <c r="F152" s="23"/>
+      <c r="G152" s="23"/>
+      <c r="H152" s="23"/>
+      <c r="I152" s="23"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="23"/>
+      <c r="B153" s="23"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="23"/>
+      <c r="E153" s="23"/>
+      <c r="F153" s="23"/>
+      <c r="G153" s="23"/>
+      <c r="H153" s="23"/>
+      <c r="I153" s="23"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="23"/>
+      <c r="B154" s="23"/>
+      <c r="C154" s="23"/>
+      <c r="D154" s="23"/>
+      <c r="E154" s="23"/>
+      <c r="F154" s="23"/>
+      <c r="G154" s="23"/>
+      <c r="H154" s="23"/>
+      <c r="I154" s="23"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="23"/>
+      <c r="B155" s="23"/>
+      <c r="C155" s="23"/>
+      <c r="D155" s="23"/>
+      <c r="E155" s="23"/>
+      <c r="F155" s="23"/>
+      <c r="G155" s="23"/>
+      <c r="H155" s="23"/>
+      <c r="I155" s="23"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="23"/>
+      <c r="B156" s="23"/>
+      <c r="C156" s="23"/>
+      <c r="D156" s="23"/>
+      <c r="E156" s="23"/>
+      <c r="F156" s="23"/>
+      <c r="G156" s="23"/>
+      <c r="H156" s="23"/>
+      <c r="I156" s="23"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="23"/>
+      <c r="B157" s="23"/>
+      <c r="C157" s="23"/>
+      <c r="D157" s="23"/>
+      <c r="E157" s="23"/>
+      <c r="F157" s="23"/>
+      <c r="G157" s="23"/>
+      <c r="H157" s="23"/>
+      <c r="I157" s="23"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="23"/>
+      <c r="B158" s="23"/>
+      <c r="C158" s="23"/>
+      <c r="D158" s="23"/>
+      <c r="E158" s="23"/>
+      <c r="F158" s="23"/>
+      <c r="G158" s="23"/>
+      <c r="H158" s="23"/>
+      <c r="I158" s="23"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="23"/>
+      <c r="B159" s="23"/>
+      <c r="C159" s="23"/>
+      <c r="D159" s="23"/>
+      <c r="E159" s="23"/>
+      <c r="F159" s="23"/>
+      <c r="G159" s="23"/>
+      <c r="H159" s="23"/>
+      <c r="I159" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A32:E32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Broke the BOM into individual files for Bob and Geoff to order stuff
</commit_message>
<xml_diff>
--- a/Design/BOM.xlsx
+++ b/Design/BOM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +262,54 @@
   </si>
   <si>
     <t>http://www.abelectronics.co.uk/products/3/Raspberry-Pi/37/Buffer-Pi</t>
+  </si>
+  <si>
+    <t>10 foot lengths</t>
+  </si>
+  <si>
+    <t>cut1</t>
+  </si>
+  <si>
+    <t>cut2</t>
+  </si>
+  <si>
+    <t>cut3</t>
+  </si>
+  <si>
+    <t>cut4</t>
+  </si>
+  <si>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>cut5</t>
+  </si>
+  <si>
+    <t>cut6</t>
+  </si>
+  <si>
+    <t>2x2 total</t>
+  </si>
+  <si>
+    <t>3x3 total</t>
+  </si>
+  <si>
+    <t>3x6 total</t>
+  </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>cut7</t>
+  </si>
+  <si>
+    <t>cut8</t>
+  </si>
+  <si>
+    <t>cut9</t>
+  </si>
+  <si>
+    <t>cut10</t>
   </si>
 </sst>
 </file>
@@ -901,7 +949,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -990,6 +1038,7 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,7 +1183,7 @@
                   <c:v>491.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>565.43395833333329</c:v>
+                  <c:v>545.26729166666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1491,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,15 +1590,15 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="79"/>
       <c r="I3" s="20">
         <f>SUM(H4:H17)</f>
         <v>630.52</v>
@@ -1655,7 +1704,7 @@
       </c>
       <c r="M6" s="38">
         <f>I44</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1686,7 +1735,7 @@
       </c>
       <c r="M7" s="22">
         <f>SUM(M3:M6)</f>
-        <v>3363.6339583333329</v>
+        <v>3343.4672916666664</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -1901,15 +1950,15 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="82"/>
       <c r="I18" s="45">
         <f>SUM(H19:H33)</f>
         <v>1676.1599999999999</v>
@@ -2244,31 +2293,31 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="82"/>
       <c r="I34" s="45">
         <f>SUM(H35:H43)</f>
         <v>491.52</v>
       </c>
-      <c r="M34" s="82" t="s">
+      <c r="M34" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N34" s="83"/>
-      <c r="O34" s="84"/>
+      <c r="N34" s="84"/>
+      <c r="O34" s="85"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D35" s="53" t="s">
         <v>50</v>
@@ -2286,11 +2335,11 @@
         <f>(E35*F35)+G35</f>
         <v>191.52</v>
       </c>
-      <c r="M35" s="82" t="s">
+      <c r="M35" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="N35" s="83"/>
-      <c r="O35" s="84"/>
+      <c r="N35" s="84"/>
+      <c r="O35" s="85"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="26" t="s">
@@ -2365,7 +2414,9 @@
       <c r="N38" s="32">
         <v>32</v>
       </c>
-      <c r="O38" s="32"/>
+      <c r="O38" s="32">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="26"/>
@@ -2386,7 +2437,9 @@
       <c r="N39" s="32">
         <v>65</v>
       </c>
-      <c r="O39" s="32"/>
+      <c r="O39" s="32">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="26"/>
@@ -2407,7 +2460,9 @@
       <c r="N40" s="32">
         <v>65</v>
       </c>
-      <c r="O40" s="32"/>
+      <c r="O40" s="32">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="26"/>
@@ -2428,7 +2483,9 @@
       <c r="N41" s="32">
         <v>73.5</v>
       </c>
-      <c r="O41" s="32"/>
+      <c r="O41" s="32">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="26"/>
@@ -2467,24 +2524,22 @@
       <c r="M43" s="32">
         <v>8</v>
       </c>
-      <c r="N43" s="32">
-        <v>120</v>
-      </c>
+      <c r="N43" s="32"/>
       <c r="O43" s="32"/>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="79" t="s">
+      <c r="B44" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="81"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="82"/>
       <c r="I44" s="45">
         <f>SUM(H45:H58)</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="M44" s="32">
         <v>8</v>
@@ -2527,7 +2582,7 @@
         <v>2x2x 1/8</v>
       </c>
       <c r="C46" s="61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="36">
@@ -2557,12 +2612,12 @@
         <v>3x3x 1/8</v>
       </c>
       <c r="C47" s="61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="36">
         <f>N51</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="F47" s="25">
         <f>(87/24)</f>
@@ -2573,7 +2628,7 @@
       </c>
       <c r="H47" s="27">
         <f t="shared" ref="H47:H48" si="4">F47*E47</f>
-        <v>139.26041666666666</v>
+        <v>103.01041666666667</v>
       </c>
       <c r="M47" s="32">
         <v>16</v>
@@ -2587,12 +2642,12 @@
         <v>3x6x 3/16</v>
       </c>
       <c r="C48" s="61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="36">
         <f>O51</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
       <c r="F48" s="25">
         <f>(193/24)*1.5</f>
@@ -2603,7 +2658,7 @@
       </c>
       <c r="H48" s="27">
         <f t="shared" si="4"/>
-        <v>57.296875</v>
+        <v>73.380208333333329</v>
       </c>
       <c r="M48" s="32">
         <v>16</v>
@@ -2611,7 +2666,7 @@
       <c r="N48" s="32"/>
       <c r="O48" s="32"/>
     </row>
-    <row r="49" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>40</v>
       </c>
@@ -2639,7 +2694,7 @@
       <c r="N49" s="32"/>
       <c r="O49" s="32"/>
     </row>
-    <row r="50" spans="1:15" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="29"/>
       <c r="C50" s="60"/>
       <c r="D50" s="24"/>
@@ -2660,7 +2715,7 @@
       <c r="N50" s="33"/>
       <c r="O50" s="33"/>
     </row>
-    <row r="51" spans="1:15" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="31"/>
       <c r="C51" s="61"/>
       <c r="D51" s="24"/>
@@ -2681,14 +2736,14 @@
       </c>
       <c r="N51" s="34">
         <f>SUM(N37:N50)/12</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="O51" s="34">
         <f>SUM(O37:O50)/12</f>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.083333333333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B52" s="26" t="s">
         <v>19</v>
       </c>
@@ -2710,12 +2765,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B53" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D53" s="28" t="s">
         <v>52</v>
@@ -2733,8 +2788,20 @@
         <f t="shared" si="5"/>
         <v>185.21</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L53" t="s">
+        <v>79</v>
+      </c>
+      <c r="N53" t="s">
+        <v>87</v>
+      </c>
+      <c r="O53" t="s">
+        <v>88</v>
+      </c>
+      <c r="P53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B54" s="26"/>
       <c r="C54" s="58"/>
       <c r="D54" s="24"/>
@@ -2747,8 +2814,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>80</v>
+      </c>
+      <c r="L54">
+        <f>(M37+M38+M39)/12</f>
+        <v>7.5</v>
+      </c>
+      <c r="M54" t="s">
+        <v>84</v>
+      </c>
+      <c r="N54">
+        <f>L54+L55+L56</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B55" s="26"/>
       <c r="C55" s="58"/>
       <c r="D55" s="24"/>
@@ -2761,8 +2842,18 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>81</v>
+      </c>
+      <c r="L55">
+        <f>(M40+M41+M42)/12</f>
+        <v>7.5</v>
+      </c>
+      <c r="M55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B56" s="26"/>
       <c r="C56" s="58"/>
       <c r="D56" s="24"/>
@@ -2775,8 +2866,18 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>82</v>
+      </c>
+      <c r="L56">
+        <f>(M43+M44+M45+M46+M47+M48+M49+M50)/12</f>
+        <v>8</v>
+      </c>
+      <c r="M56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B57" s="26"/>
       <c r="C57" s="58"/>
       <c r="D57" s="24"/>
@@ -2789,8 +2890,18 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K57" t="s">
+        <v>83</v>
+      </c>
+      <c r="L57" s="76">
+        <f>(N37+N39)/12</f>
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="M57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="62"/>
       <c r="D58" s="8"/>
@@ -2803,6 +2914,58 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="K58" t="s">
+        <v>85</v>
+      </c>
+      <c r="L58" s="76">
+        <f>(N38+N40)/12</f>
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="M58" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>86</v>
+      </c>
+      <c r="L59" s="76">
+        <f>(N41)/12</f>
+        <v>6.125</v>
+      </c>
+      <c r="M59" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K60" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="L60" s="76">
+        <f>N42/12</f>
+        <v>6.125</v>
+      </c>
+      <c r="M60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K61" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="L61" s="76"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K62" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="L62" s="76"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K63" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="L63" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4380,7 +4543,7 @@
       </c>
       <c r="B36" s="23" t="str">
         <f>Main!C35</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C36" s="23" t="str">
         <f>Main!D35</f>
@@ -4864,7 +5027,7 @@
       </c>
       <c r="B47" s="23" t="str">
         <f>Main!C46</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C47" s="23">
         <f>Main!D46</f>
@@ -4908,7 +5071,7 @@
       </c>
       <c r="B48" s="23" t="str">
         <f>Main!C47</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C48" s="23">
         <f>Main!D47</f>
@@ -4916,7 +5079,7 @@
       </c>
       <c r="D48" s="23">
         <f>Main!E47</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="E48" s="23">
         <f>Main!F47</f>
@@ -4928,7 +5091,7 @@
       </c>
       <c r="G48" s="23">
         <f>Main!H47</f>
-        <v>139.26041666666666</v>
+        <v>103.01041666666667</v>
       </c>
       <c r="H48" s="23"/>
       <c r="I48" s="23"/>
@@ -4952,7 +5115,7 @@
       </c>
       <c r="B49" s="23" t="str">
         <f>Main!C48</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C49" s="23">
         <f>Main!D48</f>
@@ -4960,7 +5123,7 @@
       </c>
       <c r="D49" s="23">
         <f>Main!E48</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
       <c r="E49" s="23">
         <f>Main!F48</f>
@@ -4972,7 +5135,7 @@
       </c>
       <c r="G49" s="23">
         <f>Main!H48</f>
-        <v>57.296875</v>
+        <v>73.380208333333329</v>
       </c>
       <c r="H49" s="23"/>
       <c r="I49" s="23"/>
@@ -5172,7 +5335,7 @@
       </c>
       <c r="B54" s="23" t="str">
         <f>Main!C53</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C54" s="23" t="str">
         <f>Main!D53</f>
@@ -9316,7 +9479,7 @@
       </c>
       <c r="L6" s="23">
         <f>Main!M6</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="M6" s="23">
         <f>Main!N6</f>
@@ -9378,7 +9541,7 @@
       </c>
       <c r="L7" s="23">
         <f>Main!M7</f>
-        <v>3363.6339583333329</v>
+        <v>3343.4672916666664</v>
       </c>
       <c r="M7" s="23">
         <f>Main!N7</f>
@@ -10438,7 +10601,7 @@
       </c>
       <c r="B25" s="23" t="str">
         <f>Main!C35</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C25" s="23" t="str">
         <f>Main!D35</f>
@@ -10556,7 +10719,7 @@
       </c>
       <c r="B28" s="23" t="str">
         <f>Main!C46</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C28" s="23">
         <f>Main!D46</f>
@@ -10586,7 +10749,7 @@
       </c>
       <c r="B29" s="23" t="str">
         <f>Main!C47</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C29" s="23">
         <f>Main!D47</f>
@@ -10594,7 +10757,7 @@
       </c>
       <c r="D29" s="23">
         <f>Main!E47</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="E29" s="63">
         <f>Main!F47</f>
@@ -10606,7 +10769,7 @@
       </c>
       <c r="G29" s="63">
         <f>Main!H47</f>
-        <v>139.26041666666666</v>
+        <v>103.01041666666667</v>
       </c>
     </row>
     <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -10790,7 +10953,7 @@
       </c>
       <c r="B33" s="23" t="str">
         <f>Main!C48</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C33" s="23">
         <f>Main!D48</f>
@@ -10798,7 +10961,7 @@
       </c>
       <c r="D33" s="23">
         <f>Main!E48</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
       <c r="E33" s="63">
         <f>Main!F48</f>
@@ -10810,7 +10973,7 @@
       </c>
       <c r="G33" s="63">
         <f>Main!H48</f>
-        <v>57.296875</v>
+        <v>73.380208333333329</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -10820,7 +10983,7 @@
       </c>
       <c r="B34" s="23" t="str">
         <f>Main!C53</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C34" s="23" t="str">
         <f>Main!D53</f>
@@ -10956,7 +11119,7 @@
       </c>
       <c r="N36" s="23">
         <f>Main!O38</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -11014,7 +11177,7 @@
       </c>
       <c r="N37" s="23">
         <f>Main!O39</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -11072,7 +11235,7 @@
       </c>
       <c r="N38" s="23">
         <f>Main!O40</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -11130,7 +11293,7 @@
       </c>
       <c r="N39" s="23">
         <f>Main!O41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -11242,7 +11405,7 @@
       </c>
       <c r="M41" s="23">
         <f>Main!N43</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="N41" s="23">
         <f>Main!O43</f>
@@ -11280,7 +11443,7 @@
       </c>
       <c r="H42" s="23">
         <f>Main!I44</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="I42" s="23">
         <f>Main!J44</f>
@@ -11722,11 +11885,11 @@
       </c>
       <c r="M49" s="23">
         <f>Main!N51</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="N49" s="23">
         <f>Main!O51</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
     </row>
     <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -11832,21 +11995,21 @@
         <f>Main!K53</f>
         <v>0</v>
       </c>
-      <c r="K51" s="23">
+      <c r="K51" s="23" t="str">
         <f>Main!L53</f>
-        <v>0</v>
+        <v>10 foot lengths</v>
       </c>
       <c r="L51" s="23">
         <f>Main!M53</f>
         <v>0</v>
       </c>
-      <c r="M51" s="23">
+      <c r="M51" s="23" t="str">
         <f>Main!N53</f>
-        <v>0</v>
-      </c>
-      <c r="N51" s="23">
+        <v>2x2 total</v>
+      </c>
+      <c r="N51" s="23" t="str">
         <f>Main!O53</f>
-        <v>0</v>
+        <v>3x3 total</v>
       </c>
       <c r="Q51" s="23" t="str">
         <f t="shared" si="4"/>
@@ -11890,21 +12053,21 @@
         <f>Main!J54</f>
         <v>0</v>
       </c>
-      <c r="J52" s="23">
+      <c r="J52" s="23" t="str">
         <f>Main!K54</f>
-        <v>0</v>
+        <v>cut1</v>
       </c>
       <c r="K52" s="23">
         <f>Main!L54</f>
-        <v>0</v>
-      </c>
-      <c r="L52" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="L52" s="23" t="str">
         <f>Main!M54</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M52" s="23">
         <f>Main!N54</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N52" s="23">
         <f>Main!O54</f>
@@ -11948,17 +12111,17 @@
         <f>Main!J55</f>
         <v>0</v>
       </c>
-      <c r="J53" s="23">
+      <c r="J53" s="23" t="str">
         <f>Main!K55</f>
-        <v>0</v>
+        <v>cut2</v>
       </c>
       <c r="K53" s="23">
         <f>Main!L55</f>
-        <v>0</v>
-      </c>
-      <c r="L53" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="L53" s="23" t="str">
         <f>Main!M55</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M53" s="23">
         <f>Main!N55</f>
@@ -12006,17 +12169,17 @@
         <f>Main!J56</f>
         <v>0</v>
       </c>
-      <c r="J54" s="23">
+      <c r="J54" s="23" t="str">
         <f>Main!K56</f>
-        <v>0</v>
+        <v>cut3</v>
       </c>
       <c r="K54" s="23">
         <f>Main!L56</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="23">
+        <v>8</v>
+      </c>
+      <c r="L54" s="23" t="str">
         <f>Main!M56</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M54" s="23">
         <f>Main!N56</f>
@@ -12064,17 +12227,17 @@
         <f>Main!J57</f>
         <v>0</v>
       </c>
-      <c r="J55" s="23">
+      <c r="J55" s="23" t="str">
         <f>Main!K57</f>
-        <v>0</v>
+        <v>cut4</v>
       </c>
       <c r="K55" s="23">
         <f>Main!L57</f>
-        <v>0</v>
-      </c>
-      <c r="L55" s="23">
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="L55" s="23" t="str">
         <f>Main!M57</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M55" s="23">
         <f>Main!N57</f>
@@ -12122,17 +12285,17 @@
         <f>Main!J58</f>
         <v>0</v>
       </c>
-      <c r="J56" s="23">
+      <c r="J56" s="23" t="str">
         <f>Main!K58</f>
-        <v>0</v>
+        <v>cut5</v>
       </c>
       <c r="K56" s="23">
         <f>Main!L58</f>
-        <v>0</v>
-      </c>
-      <c r="L56" s="23">
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="L56" s="23" t="str">
         <f>Main!M58</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M56" s="23">
         <f>Main!N58</f>
@@ -12180,17 +12343,17 @@
         <f>Main!J59</f>
         <v>0</v>
       </c>
-      <c r="J57" s="23">
+      <c r="J57" s="23" t="str">
         <f>Main!K59</f>
-        <v>0</v>
+        <v>cut6</v>
       </c>
       <c r="K57" s="23">
         <f>Main!L59</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="23">
+        <v>6.125</v>
+      </c>
+      <c r="L57" s="23" t="str">
         <f>Main!M59</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M57" s="23">
         <f>Main!N59</f>
@@ -12238,17 +12401,17 @@
         <f>Main!J60</f>
         <v>0</v>
       </c>
-      <c r="J58" s="23">
+      <c r="J58" s="23" t="str">
         <f>Main!K60</f>
-        <v>0</v>
+        <v>cut7</v>
       </c>
       <c r="K58" s="23">
         <f>Main!L60</f>
-        <v>0</v>
-      </c>
-      <c r="L58" s="23">
+        <v>6.125</v>
+      </c>
+      <c r="L58" s="23" t="str">
         <f>Main!M60</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M58" s="23">
         <f>Main!N60</f>
@@ -12296,9 +12459,9 @@
         <f>Main!J61</f>
         <v>0</v>
       </c>
-      <c r="J59" s="23">
+      <c r="J59" s="23" t="str">
         <f>Main!K61</f>
-        <v>0</v>
+        <v>cut8</v>
       </c>
       <c r="K59" s="23">
         <f>Main!L61</f>
@@ -12354,9 +12517,9 @@
         <f>Main!J62</f>
         <v>0</v>
       </c>
-      <c r="J60" s="23">
+      <c r="J60" s="23" t="str">
         <f>Main!K62</f>
-        <v>0</v>
+        <v>cut9</v>
       </c>
       <c r="K60" s="23">
         <f>Main!L62</f>
@@ -12412,9 +12575,9 @@
         <f>Main!J63</f>
         <v>0</v>
       </c>
-      <c r="J61" s="23">
+      <c r="J61" s="23" t="str">
         <f>Main!K63</f>
-        <v>0</v>
+        <v>cut10</v>
       </c>
       <c r="K61" s="23">
         <f>Main!L63</f>
@@ -17340,7 +17503,7 @@
       </c>
       <c r="L6" s="23">
         <f>Main!M6</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="M6" s="23">
         <f>Main!N6</f>
@@ -17402,7 +17565,7 @@
       </c>
       <c r="L7" s="23">
         <f>Main!M7</f>
-        <v>3363.6339583333329</v>
+        <v>3343.4672916666664</v>
       </c>
       <c r="M7" s="23">
         <f>Main!N7</f>
@@ -18206,7 +18369,7 @@
       </c>
       <c r="B25" s="23" t="str">
         <f>Main!C35</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C25" s="23" t="str">
         <f>Main!D35</f>
@@ -18258,7 +18421,7 @@
       </c>
       <c r="Q25" s="23" t="str">
         <f t="shared" ref="Q25" si="2">B25</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -18388,7 +18551,7 @@
       </c>
       <c r="B28" s="23" t="str">
         <f>Main!C46</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C28" s="23">
         <f>Main!D46</f>
@@ -18440,7 +18603,7 @@
       </c>
       <c r="Q28" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -18450,7 +18613,7 @@
       </c>
       <c r="B29" s="23" t="str">
         <f>Main!C47</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C29" s="23">
         <f>Main!D47</f>
@@ -18458,7 +18621,7 @@
       </c>
       <c r="D29" s="23">
         <f>Main!E47</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="E29" s="23">
         <f>Main!F47</f>
@@ -18470,7 +18633,7 @@
       </c>
       <c r="G29" s="23">
         <f>Main!H47</f>
-        <v>139.26041666666666</v>
+        <v>103.01041666666667</v>
       </c>
       <c r="H29" s="23">
         <f>Main!I47</f>
@@ -18502,7 +18665,7 @@
       </c>
       <c r="Q29" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -18686,7 +18849,7 @@
       </c>
       <c r="B33" s="23" t="str">
         <f>Main!C48</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C33" s="23">
         <f>Main!D48</f>
@@ -18694,7 +18857,7 @@
       </c>
       <c r="D33" s="23">
         <f>Main!E48</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
       <c r="E33" s="23">
         <f>Main!F48</f>
@@ -18706,7 +18869,7 @@
       </c>
       <c r="G33" s="23">
         <f>Main!H48</f>
-        <v>57.296875</v>
+        <v>73.380208333333329</v>
       </c>
       <c r="H33" s="23">
         <f>Main!I48</f>
@@ -18738,7 +18901,7 @@
       </c>
       <c r="Q33" s="23" t="str">
         <f t="shared" ref="Q33:Q34" si="4">B33</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -18748,7 +18911,7 @@
       </c>
       <c r="B34" s="23" t="str">
         <f>Main!C53</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C34" s="23" t="str">
         <f>Main!D53</f>
@@ -18800,7 +18963,7 @@
       </c>
       <c r="Q34" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -18916,7 +19079,7 @@
       </c>
       <c r="N36" s="23">
         <f>Main!O38</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -18974,7 +19137,7 @@
       </c>
       <c r="N37" s="23">
         <f>Main!O39</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -19032,7 +19195,7 @@
       </c>
       <c r="N38" s="23">
         <f>Main!O40</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -19090,7 +19253,7 @@
       </c>
       <c r="N39" s="23">
         <f>Main!O41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -19202,7 +19365,7 @@
       </c>
       <c r="M41" s="23">
         <f>Main!N43</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="N41" s="23">
         <f>Main!O43</f>
@@ -19240,7 +19403,7 @@
       </c>
       <c r="H42" s="23">
         <f>Main!I44</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="I42" s="23">
         <f>Main!J44</f>
@@ -19682,11 +19845,11 @@
       </c>
       <c r="M49" s="23">
         <f>Main!N51</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="N49" s="23">
         <f>Main!O51</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
     </row>
     <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -19792,21 +19955,21 @@
         <f>Main!K53</f>
         <v>0</v>
       </c>
-      <c r="K51" s="23">
+      <c r="K51" s="23" t="str">
         <f>Main!L53</f>
-        <v>0</v>
+        <v>10 foot lengths</v>
       </c>
       <c r="L51" s="23">
         <f>Main!M53</f>
         <v>0</v>
       </c>
-      <c r="M51" s="23">
+      <c r="M51" s="23" t="str">
         <f>Main!N53</f>
-        <v>0</v>
-      </c>
-      <c r="N51" s="23">
+        <v>2x2 total</v>
+      </c>
+      <c r="N51" s="23" t="str">
         <f>Main!O53</f>
-        <v>0</v>
+        <v>3x3 total</v>
       </c>
       <c r="Q51" s="23" t="str">
         <f t="shared" si="6"/>
@@ -19850,21 +20013,21 @@
         <f>Main!J54</f>
         <v>0</v>
       </c>
-      <c r="J52" s="23">
+      <c r="J52" s="23" t="str">
         <f>Main!K54</f>
-        <v>0</v>
+        <v>cut1</v>
       </c>
       <c r="K52" s="23">
         <f>Main!L54</f>
-        <v>0</v>
-      </c>
-      <c r="L52" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="L52" s="23" t="str">
         <f>Main!M54</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M52" s="23">
         <f>Main!N54</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N52" s="23">
         <f>Main!O54</f>
@@ -19908,17 +20071,17 @@
         <f>Main!J55</f>
         <v>0</v>
       </c>
-      <c r="J53" s="23">
+      <c r="J53" s="23" t="str">
         <f>Main!K55</f>
-        <v>0</v>
+        <v>cut2</v>
       </c>
       <c r="K53" s="23">
         <f>Main!L55</f>
-        <v>0</v>
-      </c>
-      <c r="L53" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="L53" s="23" t="str">
         <f>Main!M55</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M53" s="23">
         <f>Main!N55</f>
@@ -19966,17 +20129,17 @@
         <f>Main!J56</f>
         <v>0</v>
       </c>
-      <c r="J54" s="23">
+      <c r="J54" s="23" t="str">
         <f>Main!K56</f>
-        <v>0</v>
+        <v>cut3</v>
       </c>
       <c r="K54" s="23">
         <f>Main!L56</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="23">
+        <v>8</v>
+      </c>
+      <c r="L54" s="23" t="str">
         <f>Main!M56</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M54" s="23">
         <f>Main!N56</f>
@@ -20024,17 +20187,17 @@
         <f>Main!J57</f>
         <v>0</v>
       </c>
-      <c r="J55" s="23">
+      <c r="J55" s="23" t="str">
         <f>Main!K57</f>
-        <v>0</v>
+        <v>cut4</v>
       </c>
       <c r="K55" s="23">
         <f>Main!L57</f>
-        <v>0</v>
-      </c>
-      <c r="L55" s="23">
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="L55" s="23" t="str">
         <f>Main!M57</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M55" s="23">
         <f>Main!N57</f>
@@ -20082,17 +20245,17 @@
         <f>Main!J58</f>
         <v>0</v>
       </c>
-      <c r="J56" s="23">
+      <c r="J56" s="23" t="str">
         <f>Main!K58</f>
-        <v>0</v>
+        <v>cut5</v>
       </c>
       <c r="K56" s="23">
         <f>Main!L58</f>
-        <v>0</v>
-      </c>
-      <c r="L56" s="23">
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="L56" s="23" t="str">
         <f>Main!M58</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M56" s="23">
         <f>Main!N58</f>
@@ -20140,17 +20303,17 @@
         <f>Main!J59</f>
         <v>0</v>
       </c>
-      <c r="J57" s="23">
+      <c r="J57" s="23" t="str">
         <f>Main!K59</f>
-        <v>0</v>
+        <v>cut6</v>
       </c>
       <c r="K57" s="23">
         <f>Main!L59</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="23">
+        <v>6.125</v>
+      </c>
+      <c r="L57" s="23" t="str">
         <f>Main!M59</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M57" s="23">
         <f>Main!N59</f>
@@ -20198,17 +20361,17 @@
         <f>Main!J60</f>
         <v>0</v>
       </c>
-      <c r="J58" s="23">
+      <c r="J58" s="23" t="str">
         <f>Main!K60</f>
-        <v>0</v>
+        <v>cut7</v>
       </c>
       <c r="K58" s="23">
         <f>Main!L60</f>
-        <v>0</v>
-      </c>
-      <c r="L58" s="23">
+        <v>6.125</v>
+      </c>
+      <c r="L58" s="23" t="str">
         <f>Main!M60</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M58" s="23">
         <f>Main!N60</f>
@@ -20256,9 +20419,9 @@
         <f>Main!J61</f>
         <v>0</v>
       </c>
-      <c r="J59" s="23">
+      <c r="J59" s="23" t="str">
         <f>Main!K61</f>
-        <v>0</v>
+        <v>cut8</v>
       </c>
       <c r="K59" s="23">
         <f>Main!L61</f>
@@ -20314,9 +20477,9 @@
         <f>Main!J62</f>
         <v>0</v>
       </c>
-      <c r="J60" s="23">
+      <c r="J60" s="23" t="str">
         <f>Main!K62</f>
-        <v>0</v>
+        <v>cut9</v>
       </c>
       <c r="K60" s="23">
         <f>Main!L62</f>
@@ -20372,9 +20535,9 @@
         <f>Main!J63</f>
         <v>0</v>
       </c>
-      <c r="J61" s="23">
+      <c r="J61" s="23" t="str">
         <f>Main!K63</f>
-        <v>0</v>
+        <v>cut10</v>
       </c>
       <c r="K61" s="23">
         <f>Main!L63</f>
@@ -25301,7 +25464,7 @@
       </c>
       <c r="L6" s="23">
         <f>Main!M6</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="M6" s="23">
         <f>Main!N6</f>
@@ -25363,7 +25526,7 @@
       </c>
       <c r="L7" s="23">
         <f>Main!M7</f>
-        <v>3363.6339583333329</v>
+        <v>3343.4672916666664</v>
       </c>
       <c r="M7" s="23">
         <f>Main!N7</f>
@@ -26395,7 +26558,7 @@
       </c>
       <c r="B25" s="23" t="str">
         <f>Main!C35</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C25" s="23" t="str">
         <f>Main!D35</f>
@@ -26447,7 +26610,7 @@
       </c>
       <c r="Q25" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -26577,7 +26740,7 @@
       </c>
       <c r="B28" s="23" t="str">
         <f>Main!C46</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C28" s="23">
         <f>Main!D46</f>
@@ -26629,7 +26792,7 @@
       </c>
       <c r="Q28" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -26639,7 +26802,7 @@
       </c>
       <c r="B29" s="23" t="str">
         <f>Main!C47</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C29" s="23">
         <f>Main!D47</f>
@@ -26647,7 +26810,7 @@
       </c>
       <c r="D29" s="23">
         <f>Main!E47</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="E29" s="23">
         <f>Main!F47</f>
@@ -26659,7 +26822,7 @@
       </c>
       <c r="G29" s="23">
         <f>Main!H47</f>
-        <v>139.26041666666666</v>
+        <v>103.01041666666667</v>
       </c>
       <c r="H29" s="23">
         <f>Main!I47</f>
@@ -26691,7 +26854,7 @@
       </c>
       <c r="Q29" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -26875,7 +27038,7 @@
       </c>
       <c r="B33" s="23" t="str">
         <f>Main!C48</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C33" s="23">
         <f>Main!D48</f>
@@ -26883,7 +27046,7 @@
       </c>
       <c r="D33" s="23">
         <f>Main!E48</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
       <c r="E33" s="23">
         <f>Main!F48</f>
@@ -26895,7 +27058,7 @@
       </c>
       <c r="G33" s="23">
         <f>Main!H48</f>
-        <v>57.296875</v>
+        <v>73.380208333333329</v>
       </c>
       <c r="H33" s="23">
         <f>Main!I48</f>
@@ -26927,7 +27090,7 @@
       </c>
       <c r="Q33" s="23" t="str">
         <f t="shared" ref="Q33:Q34" si="4">B33</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -26937,7 +27100,7 @@
       </c>
       <c r="B34" s="23" t="str">
         <f>Main!C53</f>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
       <c r="C34" s="23" t="str">
         <f>Main!D53</f>
@@ -26989,7 +27152,7 @@
       </c>
       <c r="Q34" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>Mike</v>
+        <v>Geoff</v>
       </c>
     </row>
     <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -27105,7 +27268,7 @@
       </c>
       <c r="N36" s="23">
         <f>Main!O38</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -27163,7 +27326,7 @@
       </c>
       <c r="N37" s="23">
         <f>Main!O39</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -27221,7 +27384,7 @@
       </c>
       <c r="N38" s="23">
         <f>Main!O40</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -27279,7 +27442,7 @@
       </c>
       <c r="N39" s="23">
         <f>Main!O41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -27391,7 +27554,7 @@
       </c>
       <c r="M41" s="23">
         <f>Main!N43</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="N41" s="23">
         <f>Main!O43</f>
@@ -27429,7 +27592,7 @@
       </c>
       <c r="H42" s="23">
         <f>Main!I44</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="I42" s="23">
         <f>Main!J44</f>
@@ -27743,11 +27906,11 @@
       </c>
       <c r="M49" s="23">
         <f>Main!N51</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="N49" s="23">
         <f>Main!O51</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -27847,21 +28010,21 @@
         <f>Main!J54</f>
         <v>0</v>
       </c>
-      <c r="J52" s="23">
+      <c r="J52" s="23" t="str">
         <f>Main!K54</f>
-        <v>0</v>
+        <v>cut1</v>
       </c>
       <c r="K52" s="23">
         <f>Main!L54</f>
-        <v>0</v>
-      </c>
-      <c r="L52" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="L52" s="23" t="str">
         <f>Main!M54</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M52" s="23">
         <f>Main!N54</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N52" s="23">
         <f>Main!O54</f>
@@ -27905,17 +28068,17 @@
         <f>Main!J55</f>
         <v>0</v>
       </c>
-      <c r="J53" s="23">
+      <c r="J53" s="23" t="str">
         <f>Main!K55</f>
-        <v>0</v>
+        <v>cut2</v>
       </c>
       <c r="K53" s="23">
         <f>Main!L55</f>
-        <v>0</v>
-      </c>
-      <c r="L53" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="L53" s="23" t="str">
         <f>Main!M55</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M53" s="23">
         <f>Main!N55</f>
@@ -27963,17 +28126,17 @@
         <f>Main!J56</f>
         <v>0</v>
       </c>
-      <c r="J54" s="23">
+      <c r="J54" s="23" t="str">
         <f>Main!K56</f>
-        <v>0</v>
+        <v>cut3</v>
       </c>
       <c r="K54" s="23">
         <f>Main!L56</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="23">
+        <v>8</v>
+      </c>
+      <c r="L54" s="23" t="str">
         <f>Main!M56</f>
-        <v>0</v>
+        <v>2x2</v>
       </c>
       <c r="M54" s="23">
         <f>Main!N56</f>
@@ -28021,17 +28184,17 @@
         <f>Main!J57</f>
         <v>0</v>
       </c>
-      <c r="J55" s="23">
+      <c r="J55" s="23" t="str">
         <f>Main!K57</f>
-        <v>0</v>
+        <v>cut4</v>
       </c>
       <c r="K55" s="23">
         <f>Main!L57</f>
-        <v>0</v>
-      </c>
-      <c r="L55" s="23">
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="L55" s="23" t="str">
         <f>Main!M57</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M55" s="23">
         <f>Main!N57</f>
@@ -28079,17 +28242,17 @@
         <f>Main!J58</f>
         <v>0</v>
       </c>
-      <c r="J56" s="23">
+      <c r="J56" s="23" t="str">
         <f>Main!K58</f>
-        <v>0</v>
+        <v>cut5</v>
       </c>
       <c r="K56" s="23">
         <f>Main!L58</f>
-        <v>0</v>
-      </c>
-      <c r="L56" s="23">
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="L56" s="23" t="str">
         <f>Main!M58</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M56" s="23">
         <f>Main!N58</f>
@@ -28137,17 +28300,17 @@
         <f>Main!J59</f>
         <v>0</v>
       </c>
-      <c r="J57" s="23">
+      <c r="J57" s="23" t="str">
         <f>Main!K59</f>
-        <v>0</v>
+        <v>cut6</v>
       </c>
       <c r="K57" s="23">
         <f>Main!L59</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="23">
+        <v>6.125</v>
+      </c>
+      <c r="L57" s="23" t="str">
         <f>Main!M59</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M57" s="23">
         <f>Main!N59</f>
@@ -28195,17 +28358,17 @@
         <f>Main!J60</f>
         <v>0</v>
       </c>
-      <c r="J58" s="23">
+      <c r="J58" s="23" t="str">
         <f>Main!K60</f>
-        <v>0</v>
+        <v>cut7</v>
       </c>
       <c r="K58" s="23">
         <f>Main!L60</f>
-        <v>0</v>
-      </c>
-      <c r="L58" s="23">
+        <v>6.125</v>
+      </c>
+      <c r="L58" s="23" t="str">
         <f>Main!M60</f>
-        <v>0</v>
+        <v>3x3</v>
       </c>
       <c r="M58" s="23">
         <f>Main!N60</f>
@@ -28253,9 +28416,9 @@
         <f>Main!J61</f>
         <v>0</v>
       </c>
-      <c r="J59" s="23">
+      <c r="J59" s="23" t="str">
         <f>Main!K61</f>
-        <v>0</v>
+        <v>cut8</v>
       </c>
       <c r="K59" s="23">
         <f>Main!L61</f>
@@ -28311,9 +28474,9 @@
         <f>Main!J62</f>
         <v>0</v>
       </c>
-      <c r="J60" s="23">
+      <c r="J60" s="23" t="str">
         <f>Main!K62</f>
-        <v>0</v>
+        <v>cut9</v>
       </c>
       <c r="K60" s="23">
         <f>Main!L62</f>
@@ -28369,9 +28532,9 @@
         <f>Main!J63</f>
         <v>0</v>
       </c>
-      <c r="J61" s="23">
+      <c r="J61" s="23" t="str">
         <f>Main!K63</f>
-        <v>0</v>
+        <v>cut10</v>
       </c>
       <c r="K61" s="23">
         <f>Main!L63</f>
@@ -33048,14 +33211,14 @@
       <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="85" t="str">
+      <c r="A3" s="86" t="str">
         <f>Main!B3</f>
         <v>Electronics</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="88"/>
       <c r="F3" s="73">
         <f>Main!I3</f>
         <v>630.52</v>
@@ -33170,7 +33333,7 @@
       </c>
       <c r="J6" s="67">
         <f>Main!M6</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="K6" s="23"/>
     </row>
@@ -33204,7 +33367,7 @@
       </c>
       <c r="J7" s="68">
         <f>Main!M7</f>
-        <v>3363.6339583333329</v>
+        <v>3343.4672916666664</v>
       </c>
       <c r="K7" s="23"/>
     </row>
@@ -33405,14 +33568,14 @@
       <c r="K14" s="23"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88" t="str">
+      <c r="A15" s="89" t="str">
         <f>Main!B18</f>
         <v>Hydraulics</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="90"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="91"/>
       <c r="F15" s="73">
         <f>Main!I18</f>
         <v>1676.1599999999999</v>
@@ -33760,14 +33923,14 @@
       <c r="I28" s="23"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="88" t="str">
+      <c r="A29" s="89" t="str">
         <f>Main!B34</f>
         <v>Mechanical</v>
       </c>
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="90"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="91"/>
       <c r="F29" s="73">
         <f>Main!I34</f>
         <v>491.52</v>
@@ -33829,17 +33992,17 @@
       <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="88" t="str">
+      <c r="A32" s="89" t="str">
         <f>Main!B44</f>
         <v>Raw Materials</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="90"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="91"/>
       <c r="F32" s="73">
         <f>Main!I44</f>
-        <v>565.43395833333329</v>
+        <v>545.26729166666667</v>
       </c>
       <c r="G32" s="23"/>
       <c r="H32" s="23"/>
@@ -33904,7 +34067,7 @@
       </c>
       <c r="B35" s="24">
         <f>Main!E47</f>
-        <v>38.416666666666664</v>
+        <v>28.416666666666668</v>
       </c>
       <c r="C35" s="72">
         <f>Main!F47</f>
@@ -33916,7 +34079,7 @@
       </c>
       <c r="E35" s="72">
         <f>Main!H47</f>
-        <v>139.26041666666666</v>
+        <v>103.01041666666667</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
@@ -33930,7 +34093,7 @@
       </c>
       <c r="B36" s="24">
         <f>Main!E48</f>
-        <v>4.75</v>
+        <v>6.083333333333333</v>
       </c>
       <c r="C36" s="72">
         <f>Main!F48</f>
@@ -33942,7 +34105,7 @@
       </c>
       <c r="E36" s="72">
         <f>Main!H48</f>
-        <v>57.296875</v>
+        <v>73.380208333333329</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>

</xml_diff>